<commit_message>
Data Collection: PS4, PS3, XBOX
</commit_message>
<xml_diff>
--- a/Video Games.xlsx
+++ b/Video Games.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Video-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BD4145-177E-45B8-ABA7-6C02C1E83BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D161D80-A7FA-405B-8E13-F7773621B1E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
   </bookViews>
   <sheets>
     <sheet name="VideoGames" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Console</t>
-  </si>
-  <si>
     <t>Exclusive</t>
   </si>
   <si>
@@ -208,16 +205,433 @@
   </si>
   <si>
     <t>Closed ranged combat, typically one-on-one fights or against groups of enemies</t>
+  </si>
+  <si>
+    <t>Maneater</t>
+  </si>
+  <si>
+    <t>Tripwire Interactive</t>
+  </si>
+  <si>
+    <t>Playstation 4</t>
+  </si>
+  <si>
+    <t>Horizon Zero Dawn Complete Edition</t>
+  </si>
+  <si>
+    <t>Guerilla Games</t>
+  </si>
+  <si>
+    <t>Destiny 2</t>
+  </si>
+  <si>
+    <t>Bungie Inc</t>
+  </si>
+  <si>
+    <t>The Division 2</t>
+  </si>
+  <si>
+    <t>Massive Entertainment</t>
+  </si>
+  <si>
+    <t>The Last of Us Part 2</t>
+  </si>
+  <si>
+    <t>Naughty Dog</t>
+  </si>
+  <si>
+    <t>Call of Duty Modern Warfare</t>
+  </si>
+  <si>
+    <t>Infinity Ward</t>
+  </si>
+  <si>
+    <t>Call of Duty Advanced Warfare</t>
+  </si>
+  <si>
+    <t>Sledgehammer Games</t>
+  </si>
+  <si>
+    <t>Battlefield 4</t>
+  </si>
+  <si>
+    <t>Naruto Shippuden Ultimate Ninja Storm 4</t>
+  </si>
+  <si>
+    <t>CyberConnect2</t>
+  </si>
+  <si>
+    <t>Call of Duty Black Ops 3</t>
+  </si>
+  <si>
+    <t>Treyarch</t>
+  </si>
+  <si>
+    <t>Call of Duty Black Ops 4</t>
+  </si>
+  <si>
+    <t>Far Cry 5</t>
+  </si>
+  <si>
+    <t>3/27/20118</t>
+  </si>
+  <si>
+    <t>Ubisoft Montreal</t>
+  </si>
+  <si>
+    <t>Ratchet and Clank</t>
+  </si>
+  <si>
+    <t>Insomniac Games</t>
+  </si>
+  <si>
+    <t>Call of Duty WWII</t>
+  </si>
+  <si>
+    <t>Overwatch Origins Edition</t>
+  </si>
+  <si>
+    <t>Blizzard Entertainment</t>
+  </si>
+  <si>
+    <t>Lego Star Wars The Force Awakens</t>
+  </si>
+  <si>
+    <t>TT Games</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny </t>
+  </si>
+  <si>
+    <t>Lego Marvel's Avengers</t>
+  </si>
+  <si>
+    <t>Battlefield 1</t>
+  </si>
+  <si>
+    <t>Playstation 3</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Ghost Recon Future Soldier</t>
+  </si>
+  <si>
+    <t>Red Storm Entertainment</t>
+  </si>
+  <si>
+    <t>SSX</t>
+  </si>
+  <si>
+    <t>EA Canada</t>
+  </si>
+  <si>
+    <t>Borderlands 2</t>
+  </si>
+  <si>
+    <t>Gearbox Software</t>
+  </si>
+  <si>
+    <t>Lego Star Wars III The Clone Wars</t>
+  </si>
+  <si>
+    <t>Rayman Origins</t>
+  </si>
+  <si>
+    <t>Ubisoft Montpellier</t>
+  </si>
+  <si>
+    <t>Lego Marvel Super Heroes</t>
+  </si>
+  <si>
+    <t>Split Second</t>
+  </si>
+  <si>
+    <t>Black Rock Studio</t>
+  </si>
+  <si>
+    <t>Naruto Shippuden Ultimate Ninja Storm 3</t>
+  </si>
+  <si>
+    <t>Twisted Metal</t>
+  </si>
+  <si>
+    <t>Eat Sleep Play</t>
+  </si>
+  <si>
+    <t>Street Fighter IV</t>
+  </si>
+  <si>
+    <t>Capcom</t>
+  </si>
+  <si>
+    <t>God of War III</t>
+  </si>
+  <si>
+    <t>Santa Monica Studio</t>
+  </si>
+  <si>
+    <t>Call of Duty Modern Warfare 3</t>
+  </si>
+  <si>
+    <t>Call of Duty Modern Warfare 2</t>
+  </si>
+  <si>
+    <t>Call of Duty Ghosts</t>
+  </si>
+  <si>
+    <t>Battlefield 3</t>
+  </si>
+  <si>
+    <t>DICE</t>
+  </si>
+  <si>
+    <t>Lego The Lord of the Rings</t>
+  </si>
+  <si>
+    <t>Traveller's Tales</t>
+  </si>
+  <si>
+    <t>Xbox</t>
+  </si>
+  <si>
+    <t>Conker Live and Reloaded</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Yager</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Designed to closely simulate aspects of a real or fictional reality</t>
+  </si>
+  <si>
+    <t>Yager Development</t>
+  </si>
+  <si>
+    <t>NCAA Football 2005</t>
+  </si>
+  <si>
+    <t>EA Tiburon</t>
+  </si>
+  <si>
+    <t>Oddworld Munch's Oddysee</t>
+  </si>
+  <si>
+    <t>Oddworld Inhabitants</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Galleon</t>
+  </si>
+  <si>
+    <t>Confounding Factor</t>
+  </si>
+  <si>
+    <t>Oddworld Stranger's Wrath</t>
+  </si>
+  <si>
+    <t>Armed and Dangerous</t>
+  </si>
+  <si>
+    <t>Planet Moon Studios</t>
+  </si>
+  <si>
+    <t>Prince of Persia The Sands od Time</t>
+  </si>
+  <si>
+    <t>Deus Ex Invisible War</t>
+  </si>
+  <si>
+    <t>Ion Storm</t>
+  </si>
+  <si>
+    <t>Jade Empire Limited Edition</t>
+  </si>
+  <si>
+    <t>BioWare</t>
+  </si>
+  <si>
+    <t>New Legends</t>
+  </si>
+  <si>
+    <t>Infinite Group</t>
+  </si>
+  <si>
+    <t>Crimson Sea</t>
+  </si>
+  <si>
+    <t>Koei Tecmo Games</t>
+  </si>
+  <si>
+    <t>Unreal Championship 2 The Liandri Conflict</t>
+  </si>
+  <si>
+    <t>Epic Games</t>
+  </si>
+  <si>
+    <t>Unreal Championship</t>
+  </si>
+  <si>
+    <t>The King of Fighters NeoWave</t>
+  </si>
+  <si>
+    <t>The King of Fighters 2002</t>
+  </si>
+  <si>
+    <t>The King of Fighters 2003</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Halo Combat Evolved</t>
+  </si>
+  <si>
+    <t>Halo 2 Limited Collector's Edition</t>
+  </si>
+  <si>
+    <t>Otogi Myth of Demons</t>
+  </si>
+  <si>
+    <t>FromSoftware Inc</t>
+  </si>
+  <si>
+    <t>Otogi 2 Immortal Warriors</t>
+  </si>
+  <si>
+    <t>Panzer Dragoon Orta</t>
+  </si>
+  <si>
+    <t>Sega Sports R&amp;D</t>
+  </si>
+  <si>
+    <t>Gunvalkyrie</t>
+  </si>
+  <si>
+    <t>Smilebit</t>
+  </si>
+  <si>
+    <t>Metal Slug 4</t>
+  </si>
+  <si>
+    <t>Metal Slug 5</t>
+  </si>
+  <si>
+    <t>Metal Slug 3</t>
+  </si>
+  <si>
+    <t>Wrath Unleashed</t>
+  </si>
+  <si>
+    <t>The Collective</t>
+  </si>
+  <si>
+    <t>Phantom Dust</t>
+  </si>
+  <si>
+    <t>Microsoft Game Studios</t>
+  </si>
+  <si>
+    <t>Konami</t>
+  </si>
+  <si>
+    <t>Yu-Gi-Oh The Dawn of Destiny</t>
+  </si>
+  <si>
+    <t>Magic The Gathering Battlegrounds</t>
+  </si>
+  <si>
+    <t>Sega Studios San Francisco</t>
+  </si>
+  <si>
+    <t>Bloody Roar Extreme</t>
+  </si>
+  <si>
+    <t>Eighting</t>
+  </si>
+  <si>
+    <t>Guilty Gear X2 #Reload</t>
+  </si>
+  <si>
+    <t>Arc System Works</t>
+  </si>
+  <si>
+    <t>Kakuto Chojin Back Alley Brutal</t>
+  </si>
+  <si>
+    <t>Dream Factory</t>
+  </si>
+  <si>
+    <t>Soulcalibur 2</t>
+  </si>
+  <si>
+    <t>Project Soul</t>
+  </si>
+  <si>
+    <t>Samurai Shodown V</t>
+  </si>
+  <si>
+    <t>Capcom Fighting Evolution</t>
+  </si>
+  <si>
+    <t>Capcom Production Studio 2</t>
+  </si>
+  <si>
+    <t>Capcom vs SNK 2 EO</t>
+  </si>
+  <si>
+    <t>SNK vs Capcom SVC Chaos</t>
+  </si>
+  <si>
+    <t>KOF Maximum Impact</t>
+  </si>
+  <si>
+    <t>Prince of Persia  Warrior Within</t>
+  </si>
+  <si>
+    <t>Beyond Good &amp; Evil</t>
+  </si>
+  <si>
+    <t>Brute Force</t>
+  </si>
+  <si>
+    <t>Digital Anvil</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Ghost Recon Island Thunder</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Rainbox Six 3 Black Arrow</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Rainbox Six 3</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Ghost Recon 2 2011 Final Assault</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Ghost Recon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -560,22 +974,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58CEA45-1A97-47FC-8ACE-673891E6166E}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="7" max="7" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -592,125 +1008,2004 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43973</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42794</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>A3+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42984</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:A20" si="0">A4+1</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43503</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43763</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41947</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41576</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42404</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42314</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43385</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42472</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43042</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42304</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42549</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="1">
+        <v>41891</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42395</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f>A19+1</f>
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42664</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f t="shared" ref="A21:A84" si="1">A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="1">
+        <v>41051</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="1">
+        <v>40967</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="1">
+        <v>41180</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="1">
+        <v>40624</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="1">
+        <v>40862</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="1">
+        <v>41569</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="1">
+        <v>40316</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="1">
+        <v>41338</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="1">
+        <v>40953</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="1">
+        <v>39861</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="1">
+        <v>40253</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="1">
+        <v>40855</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="1">
+        <v>40127</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="1">
+        <v>41583</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="1">
+        <v>40841</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="1">
+        <v>41212</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <f>A36+1</f>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="1">
+        <v>38524</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="1">
+        <v>38258</v>
+      </c>
+      <c r="D38" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="1">
+        <v>38183</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="1">
+        <v>37210</v>
+      </c>
+      <c r="D40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" t="s">
+        <v>127</v>
+      </c>
+      <c r="F40" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="1">
+        <v>38149</v>
+      </c>
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="1">
+        <v>111425</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="1">
+        <v>37957</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" t="s">
+        <v>133</v>
+      </c>
+      <c r="F43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="1">
+        <v>37943</v>
+      </c>
+      <c r="D44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="1">
+        <v>37957</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="1">
+        <v>38454</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="1">
+        <v>37304</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="1">
+        <v>37602</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F48" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="1">
+        <v>38460</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" t="s">
+        <v>117</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="1">
+        <v>37572</v>
+      </c>
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="1">
+        <v>38198</v>
+      </c>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" t="s">
+        <v>117</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="1">
+        <v>37539</v>
+      </c>
+      <c r="D52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="1">
+        <v>37691</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" t="s">
+        <v>117</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="1">
+        <v>37210</v>
+      </c>
+      <c r="D54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="1">
+        <v>38300</v>
+      </c>
+      <c r="D55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" s="1">
+        <v>37602</v>
+      </c>
+      <c r="D56" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" t="s">
+        <v>153</v>
+      </c>
+      <c r="F56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="1">
+        <v>37980</v>
+      </c>
+      <c r="D57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" t="s">
+        <v>153</v>
+      </c>
+      <c r="F57" t="s">
+        <v>117</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C58" s="1">
+        <v>37609</v>
+      </c>
+      <c r="D58" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58" t="s">
+        <v>156</v>
+      </c>
+      <c r="F58" t="s">
+        <v>117</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" s="1">
+        <v>37333</v>
+      </c>
+      <c r="D59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" t="s">
+        <v>158</v>
+      </c>
+      <c r="F59" t="s">
+        <v>117</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" s="1">
+        <v>37419</v>
+      </c>
+      <c r="D60" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" t="s">
+        <v>117</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="1">
+        <v>38496</v>
+      </c>
+      <c r="D61" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" t="s">
+        <v>117</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="1">
+        <v>36608</v>
+      </c>
+      <c r="D62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E62" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>162</v>
+      </c>
+      <c r="C63" s="1">
+        <v>38027</v>
+      </c>
+      <c r="D63" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+      <c r="F63" t="s">
+        <v>117</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="1">
+        <v>38253</v>
+      </c>
+      <c r="D64" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" t="s">
+        <v>165</v>
+      </c>
+      <c r="F64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="1">
+        <v>38069</v>
+      </c>
+      <c r="D65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" t="s">
+        <v>166</v>
+      </c>
+      <c r="F65" t="s">
+        <v>117</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" s="1">
+        <v>37943</v>
+      </c>
+      <c r="D66" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66" t="s">
+        <v>169</v>
+      </c>
+      <c r="F66" t="s">
+        <v>117</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C67" s="1">
+        <v>37699</v>
+      </c>
+      <c r="D67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E67" t="s">
+        <v>171</v>
+      </c>
+      <c r="F67" t="s">
+        <v>117</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="1">
+        <v>37399</v>
+      </c>
+      <c r="D68" t="s">
+        <v>48</v>
+      </c>
+      <c r="E68" t="s">
+        <v>173</v>
+      </c>
+      <c r="F68" t="s">
+        <v>117</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>174</v>
+      </c>
+      <c r="C69" s="1">
+        <v>37571</v>
+      </c>
+      <c r="D69" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" t="s">
+        <v>175</v>
+      </c>
+      <c r="F69" t="s">
+        <v>117</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="1">
+        <v>37412</v>
+      </c>
+      <c r="D70" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" t="s">
+        <v>177</v>
+      </c>
+      <c r="F70" t="s">
+        <v>117</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" s="1">
+        <v>37904</v>
+      </c>
+      <c r="D71" t="s">
+        <v>48</v>
+      </c>
+      <c r="E71" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>179</v>
+      </c>
+      <c r="C72" s="1">
+        <v>38517</v>
+      </c>
+      <c r="D72" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" t="s">
+        <v>180</v>
+      </c>
+      <c r="F72" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" s="1">
+        <v>37666</v>
+      </c>
+      <c r="D73" t="s">
+        <v>48</v>
+      </c>
+      <c r="E73" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" t="s">
+        <v>117</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>182</v>
+      </c>
+      <c r="C74" s="1">
+        <v>37826</v>
+      </c>
+      <c r="D74" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" t="s">
+        <v>117</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>183</v>
+      </c>
+      <c r="C75" s="1">
+        <v>38211</v>
+      </c>
+      <c r="D75" t="s">
+        <v>48</v>
+      </c>
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" t="s">
+        <v>117</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>184</v>
+      </c>
+      <c r="C76" s="1">
+        <v>38321</v>
+      </c>
+      <c r="D76" t="s">
+        <v>43</v>
+      </c>
+      <c r="E76" t="s">
+        <v>79</v>
+      </c>
+      <c r="F76" t="s">
+        <v>117</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" s="1">
+        <v>37936</v>
+      </c>
+      <c r="D77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E77" t="s">
+        <v>99</v>
+      </c>
+      <c r="F77" t="s">
+        <v>117</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" s="1">
+        <v>37768</v>
+      </c>
+      <c r="D78" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" t="s">
+        <v>187</v>
+      </c>
+      <c r="F78" t="s">
+        <v>117</v>
+      </c>
+      <c r="G78" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>188</v>
+      </c>
+      <c r="C79" s="1">
+        <v>37524</v>
+      </c>
+      <c r="D79" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F79" t="s">
+        <v>117</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" s="1">
+        <v>38204</v>
+      </c>
+      <c r="D80" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" t="s">
+        <v>79</v>
+      </c>
+      <c r="F80" t="s">
+        <v>117</v>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="1">
+        <v>37922</v>
+      </c>
+      <c r="D81" t="s">
+        <v>44</v>
+      </c>
+      <c r="E81" t="s">
+        <v>79</v>
+      </c>
+      <c r="F81" t="s">
+        <v>117</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>191</v>
+      </c>
+      <c r="C82" s="1">
+        <v>38307</v>
+      </c>
+      <c r="D82" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F82" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>192</v>
+      </c>
+      <c r="C83" s="1">
+        <v>37208</v>
+      </c>
+      <c r="D83" t="s">
+        <v>44</v>
+      </c>
+      <c r="E83" t="s">
+        <v>92</v>
+      </c>
+      <c r="F83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -803,7 +3098,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f t="shared" ref="A5:A20" si="0">A4+1</f>
+        <f t="shared" ref="A5:A12" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -953,10 +3248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B0A4AE-C2F8-404D-A551-5227A91C7005}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,10 +3276,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -993,22 +3288,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f t="shared" ref="A4:A18" si="0">A3+1</f>
+        <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1017,10 +3312,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1029,10 +3324,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1041,10 +3336,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1052,10 +3347,21 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +3455,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f t="shared" ref="A5:A20" si="0">A4+1</f>
+        <f t="shared" ref="A5:A6" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
Finished Xbox, 360, and Neo Geo Pocket
</commit_message>
<xml_diff>
--- a/Video Games.xlsx
+++ b/Video Games.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Video-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D161D80-A7FA-405B-8E13-F7773621B1E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB23BBA-BC82-4EC3-888D-B29F72F2030D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="300">
   <si>
     <t>Name</t>
   </si>
@@ -616,6 +616,327 @@
   </si>
   <si>
     <t>Tom Clancy's Ghost Recon</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Splinter Cell Chaos Theroy Limited Collector's Edition</t>
+  </si>
+  <si>
+    <t>Stealth</t>
+  </si>
+  <si>
+    <t>Games tend to emphasize sneaking around and avoiding enemy notice over direct conflict</t>
+  </si>
+  <si>
+    <t>Deathrow Underground Team Combat</t>
+  </si>
+  <si>
+    <t>Southend Interactive</t>
+  </si>
+  <si>
+    <t>Spikeout Battle Street</t>
+  </si>
+  <si>
+    <t>Amusement Vision</t>
+  </si>
+  <si>
+    <t>Outrun 2</t>
+  </si>
+  <si>
+    <t>Sumo Digital</t>
+  </si>
+  <si>
+    <t>Juiced</t>
+  </si>
+  <si>
+    <t>Juice Games</t>
+  </si>
+  <si>
+    <t>Steel Battalion</t>
+  </si>
+  <si>
+    <t>Steel Battalion Line of Contact</t>
+  </si>
+  <si>
+    <t>Nude Maker</t>
+  </si>
+  <si>
+    <t>Murakumo Renegade Mech Pursuit</t>
+  </si>
+  <si>
+    <t>Mech Assault 2 Lone Wolf Limited Edition</t>
+  </si>
+  <si>
+    <t>Day 1 Studios</t>
+  </si>
+  <si>
+    <t>The House of the Dead III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sega </t>
+  </si>
+  <si>
+    <t>Jet Set Radio Future</t>
+  </si>
+  <si>
+    <t>Midway Arcade Treasures 2</t>
+  </si>
+  <si>
+    <t>Backbone Entertainment</t>
+  </si>
+  <si>
+    <t>Midway Arcade Treasures 3</t>
+  </si>
+  <si>
+    <t>Hunter The Reckoning Redeemer</t>
+  </si>
+  <si>
+    <t>High Voltage Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunter The Reckoning </t>
+  </si>
+  <si>
+    <t>XIII</t>
+  </si>
+  <si>
+    <t>Breakdown</t>
+  </si>
+  <si>
+    <t>Namco</t>
+  </si>
+  <si>
+    <t>Kill Switch</t>
+  </si>
+  <si>
+    <t>Namco USA</t>
+  </si>
+  <si>
+    <t>Thief Deadly Shadows</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Splinter Cell</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Splinter Cell Pandora Tomorrow</t>
+  </si>
+  <si>
+    <t>Ubisoft Milan</t>
+  </si>
+  <si>
+    <t>BlazeBlue Calamity Trigger</t>
+  </si>
+  <si>
+    <t>Deus Ex Human Revolution</t>
+  </si>
+  <si>
+    <t>Eidos-Montreal</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Splinter Cell Blacklist</t>
+  </si>
+  <si>
+    <t>Ubisoft Toronto</t>
+  </si>
+  <si>
+    <t>Your Shape Fitness Evolved</t>
+  </si>
+  <si>
+    <t>Ubisoft</t>
+  </si>
+  <si>
+    <t>Crysis 2 Limited Edition</t>
+  </si>
+  <si>
+    <t>Crytek</t>
+  </si>
+  <si>
+    <t>Zumba Fitness Rush</t>
+  </si>
+  <si>
+    <t>Zoe Mode</t>
+  </si>
+  <si>
+    <t>Halo 3</t>
+  </si>
+  <si>
+    <t>Lost Planet Extreme Condition Collector's Edition</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Splinter Cell Conviction</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Splinter Cell Double Cell</t>
+  </si>
+  <si>
+    <t>Gears of War</t>
+  </si>
+  <si>
+    <t>Halo Wars</t>
+  </si>
+  <si>
+    <t>Ensemble Studios</t>
+  </si>
+  <si>
+    <t>Perfect Dark Zero</t>
+  </si>
+  <si>
+    <t>Prey</t>
+  </si>
+  <si>
+    <t>Human Head Studios</t>
+  </si>
+  <si>
+    <t>Kameo</t>
+  </si>
+  <si>
+    <t>WarTech Senko no Ronde</t>
+  </si>
+  <si>
+    <t>G.rev</t>
+  </si>
+  <si>
+    <t>Halo 3 ODST</t>
+  </si>
+  <si>
+    <t>Condemned Criminal Origins</t>
+  </si>
+  <si>
+    <t>Monolith Productions</t>
+  </si>
+  <si>
+    <t>Street Fighter IV Collector's Edition</t>
+  </si>
+  <si>
+    <t>Mass Effect</t>
+  </si>
+  <si>
+    <t>Condemned 2 Bloodshot</t>
+  </si>
+  <si>
+    <t>F.E.A.R.</t>
+  </si>
+  <si>
+    <t>Half-Life 2 Episode Two</t>
+  </si>
+  <si>
+    <t>Valve Corporation</t>
+  </si>
+  <si>
+    <t>Team Fortress 2</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>The Darkness</t>
+  </si>
+  <si>
+    <t>Starbreeze Studios</t>
+  </si>
+  <si>
+    <t>Rockstar Games Presents Table Tennis</t>
+  </si>
+  <si>
+    <t>Rockstar San Diego</t>
+  </si>
+  <si>
+    <t>Virtua Fighter 5</t>
+  </si>
+  <si>
+    <t>Sega AM2</t>
+  </si>
+  <si>
+    <t>Halo Combat Evolved Anniversary</t>
+  </si>
+  <si>
+    <t>343 Industries</t>
+  </si>
+  <si>
+    <t>Halo Reach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soulcaliber IV </t>
+  </si>
+  <si>
+    <t>Zone of the Enders HD Collection</t>
+  </si>
+  <si>
+    <t>Konami Computer Entertainment Japan</t>
+  </si>
+  <si>
+    <t>Halo 4</t>
+  </si>
+  <si>
+    <t>Mortal Kombat Komplete Edition</t>
+  </si>
+  <si>
+    <t>NetherRealm Studios</t>
+  </si>
+  <si>
+    <t>Kinect Adventures</t>
+  </si>
+  <si>
+    <t>Good Science Studio</t>
+  </si>
+  <si>
+    <t>Soulcaliber V</t>
+  </si>
+  <si>
+    <t>Gears of War 2</t>
+  </si>
+  <si>
+    <t>The Chronicles of Riddick Assault on Dark Athena</t>
+  </si>
+  <si>
+    <t>Samurai Shodown Sen</t>
+  </si>
+  <si>
+    <t>Project Gotham Racing 3</t>
+  </si>
+  <si>
+    <t>Bizarre Creations</t>
+  </si>
+  <si>
+    <t>Street Fighter Anniversary Collection</t>
+  </si>
+  <si>
+    <t>Sonic the Hedgehog Pocket Adventure</t>
+  </si>
+  <si>
+    <t>SNK vs Capcom The Match of the Millenium</t>
+  </si>
+  <si>
+    <t>Pac-Man</t>
+  </si>
+  <si>
+    <t>Neo Turf Masters</t>
+  </si>
+  <si>
+    <t>Saurus</t>
+  </si>
+  <si>
+    <t>King of Fighters R-2</t>
+  </si>
+  <si>
+    <t>Metal Slug 1st Mission</t>
+  </si>
+  <si>
+    <t>Ukiyotei Company Ltd</t>
+  </si>
+  <si>
+    <t>Samurai Shodown 2</t>
+  </si>
+  <si>
+    <t>Fatal Fury First Contact</t>
+  </si>
+  <si>
+    <t>The Last Blade</t>
+  </si>
+  <si>
+    <t>Aicom</t>
+  </si>
+  <si>
+    <t>Biomotor Unitron</t>
   </si>
 </sst>
 </file>
@@ -974,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58CEA45-1A97-47FC-8ACE-673891E6166E}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,7 +1308,7 @@
     <col min="3" max="3" width="12.26953125" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" customWidth="1"/>
     <col min="5" max="5" width="24.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
     <col min="7" max="7" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1089,7 +1410,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f t="shared" ref="A5:A20" si="0">A4+1</f>
+        <f t="shared" ref="A5:A19" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1473,7 +1794,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f t="shared" ref="A21:A84" si="1">A20+1</f>
+        <f t="shared" ref="A21:A85" si="1">A20+1</f>
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -2926,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2950,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -2974,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -2998,10 +3319,1810 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="1">
+        <v>38432</v>
+      </c>
+      <c r="D84" t="s">
+        <v>194</v>
+      </c>
+      <c r="E84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F84" t="s">
+        <v>117</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>196</v>
+      </c>
+      <c r="C85" s="1">
+        <v>37551</v>
+      </c>
+      <c r="D85" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" t="s">
+        <v>197</v>
+      </c>
+      <c r="F85" t="s">
+        <v>117</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <f t="shared" ref="A86:A149" si="2">A85+1</f>
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+      <c r="C86" s="1">
+        <v>38435</v>
+      </c>
+      <c r="D86" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" t="s">
+        <v>199</v>
+      </c>
+      <c r="F86" t="s">
+        <v>117</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>200</v>
+      </c>
+      <c r="C87" s="1">
+        <v>37973</v>
+      </c>
+      <c r="D87" t="s">
+        <v>47</v>
+      </c>
+      <c r="E87" t="s">
+        <v>201</v>
+      </c>
+      <c r="F87" t="s">
+        <v>117</v>
+      </c>
+      <c r="G87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>202</v>
+      </c>
+      <c r="C88" s="1">
+        <v>38516</v>
+      </c>
+      <c r="D88" t="s">
+        <v>47</v>
+      </c>
+      <c r="E88" t="s">
+        <v>203</v>
+      </c>
+      <c r="F88" t="s">
+        <v>117</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>204</v>
+      </c>
+      <c r="C89" s="1">
+        <v>37511</v>
+      </c>
+      <c r="D89" t="s">
+        <v>121</v>
+      </c>
+      <c r="E89" t="s">
+        <v>206</v>
+      </c>
+      <c r="F89" t="s">
+        <v>117</v>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>205</v>
+      </c>
+      <c r="C90" s="1">
+        <v>38043</v>
+      </c>
+      <c r="D90" t="s">
+        <v>121</v>
+      </c>
+      <c r="E90" t="s">
+        <v>206</v>
+      </c>
+      <c r="F90" t="s">
+        <v>117</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" s="1">
+        <v>37462</v>
+      </c>
+      <c r="D91" t="s">
+        <v>44</v>
+      </c>
+      <c r="E91" t="s">
+        <v>153</v>
+      </c>
+      <c r="F91" t="s">
+        <v>117</v>
+      </c>
+      <c r="G91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" s="1">
+        <v>38349</v>
+      </c>
+      <c r="D92" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" t="s">
+        <v>209</v>
+      </c>
+      <c r="F92" t="s">
+        <v>117</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>210</v>
+      </c>
+      <c r="C93" s="1">
+        <v>37408</v>
+      </c>
+      <c r="D93" t="s">
+        <v>44</v>
+      </c>
+      <c r="E93" t="s">
+        <v>211</v>
+      </c>
+      <c r="F93" t="s">
+        <v>117</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>212</v>
+      </c>
+      <c r="C94" s="1">
+        <v>37309</v>
+      </c>
+      <c r="D94" t="s">
+        <v>43</v>
+      </c>
+      <c r="E94" t="s">
+        <v>156</v>
+      </c>
+      <c r="F94" t="s">
+        <v>117</v>
+      </c>
+      <c r="G94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="1">
+        <v>38271</v>
+      </c>
+      <c r="E95" t="s">
+        <v>214</v>
+      </c>
+      <c r="F95" t="s">
+        <v>117</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" s="1">
+        <v>38622</v>
+      </c>
+      <c r="E96" t="s">
+        <v>214</v>
+      </c>
+      <c r="F96" t="s">
+        <v>117</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
+      <c r="C97" s="1">
+        <v>37922</v>
+      </c>
+      <c r="D97" t="s">
+        <v>43</v>
+      </c>
+      <c r="E97" t="s">
+        <v>217</v>
+      </c>
+      <c r="F97" t="s">
+        <v>117</v>
+      </c>
+      <c r="G97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" s="1">
+        <v>37397</v>
+      </c>
+      <c r="D98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E98" t="s">
+        <v>217</v>
+      </c>
+      <c r="F98" t="s">
+        <v>117</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>219</v>
+      </c>
+      <c r="C99" s="1">
+        <v>37943</v>
+      </c>
+      <c r="D99" t="s">
+        <v>44</v>
+      </c>
+      <c r="E99" t="s">
+        <v>197</v>
+      </c>
+      <c r="F99" t="s">
+        <v>117</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>220</v>
+      </c>
+      <c r="C100" s="1">
+        <v>38015</v>
+      </c>
+      <c r="D100" t="s">
+        <v>44</v>
+      </c>
+      <c r="E100" t="s">
+        <v>221</v>
+      </c>
+      <c r="F100" t="s">
+        <v>117</v>
+      </c>
+      <c r="G100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>222</v>
+      </c>
+      <c r="C101" s="1">
+        <v>37922</v>
+      </c>
+      <c r="D101" t="s">
+        <v>44</v>
+      </c>
+      <c r="E101" t="s">
+        <v>223</v>
+      </c>
+      <c r="F101" t="s">
+        <v>117</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>224</v>
+      </c>
+      <c r="C102" s="1">
+        <v>38132</v>
+      </c>
+      <c r="D102" t="s">
+        <v>194</v>
+      </c>
+      <c r="E102" t="s">
+        <v>136</v>
+      </c>
+      <c r="F102" t="s">
+        <v>117</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>225</v>
+      </c>
+      <c r="C103" s="1">
+        <v>37577</v>
+      </c>
+      <c r="D103" t="s">
+        <v>194</v>
+      </c>
+      <c r="E103" t="s">
+        <v>79</v>
+      </c>
+      <c r="F103" t="s">
+        <v>117</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>286</v>
+      </c>
+      <c r="C104" s="1">
+        <v>38230</v>
+      </c>
+      <c r="D104" t="s">
+        <v>48</v>
+      </c>
+      <c r="E104" t="s">
+        <v>107</v>
+      </c>
+      <c r="F104" t="s">
+        <v>117</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" s="1">
+        <v>38069</v>
+      </c>
+      <c r="D105" t="s">
+        <v>194</v>
+      </c>
+      <c r="E105" t="s">
+        <v>227</v>
+      </c>
+      <c r="F105" t="s">
+        <v>117</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" s="1">
+        <v>39994</v>
+      </c>
+      <c r="D106" t="s">
+        <v>48</v>
+      </c>
+      <c r="E106" t="s">
+        <v>173</v>
+      </c>
+      <c r="F106" t="s">
+        <v>24</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>229</v>
+      </c>
+      <c r="C107" s="1">
+        <v>40778</v>
+      </c>
+      <c r="D107" t="s">
+        <v>45</v>
+      </c>
+      <c r="E107" t="s">
+        <v>230</v>
+      </c>
+      <c r="F107" t="s">
+        <v>24</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>231</v>
+      </c>
+      <c r="C108" s="1">
+        <v>41506</v>
+      </c>
+      <c r="D108" t="s">
+        <v>194</v>
+      </c>
+      <c r="E108" t="s">
+        <v>232</v>
+      </c>
+      <c r="F108" t="s">
+        <v>24</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>233</v>
+      </c>
+      <c r="C109" s="1">
+        <v>40486</v>
+      </c>
+      <c r="E109" t="s">
+        <v>234</v>
+      </c>
+      <c r="F109" t="s">
+        <v>24</v>
+      </c>
+      <c r="G109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>235</v>
+      </c>
+      <c r="C110" s="1">
+        <v>40624</v>
+      </c>
+      <c r="D110" t="s">
+        <v>44</v>
+      </c>
+      <c r="E110" t="s">
+        <v>236</v>
+      </c>
+      <c r="F110" t="s">
+        <v>24</v>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>237</v>
+      </c>
+      <c r="C111" s="1">
+        <v>40952</v>
+      </c>
+      <c r="E111" t="s">
+        <v>238</v>
+      </c>
+      <c r="F111" t="s">
+        <v>24</v>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>239</v>
+      </c>
+      <c r="C112" s="1">
+        <v>39350</v>
+      </c>
+      <c r="D112" t="s">
+        <v>44</v>
+      </c>
+      <c r="E112" t="s">
+        <v>62</v>
+      </c>
+      <c r="F112" t="s">
+        <v>24</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>240</v>
+      </c>
+      <c r="C113" s="1">
+        <v>39072</v>
+      </c>
+      <c r="D113" t="s">
+        <v>44</v>
+      </c>
+      <c r="E113" t="s">
+        <v>107</v>
+      </c>
+      <c r="F113" t="s">
+        <v>24</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>241</v>
+      </c>
+      <c r="C114" s="1">
+        <v>40281</v>
+      </c>
+      <c r="D114" t="s">
+        <v>194</v>
+      </c>
+      <c r="E114" t="s">
+        <v>79</v>
+      </c>
+      <c r="F114" t="s">
+        <v>24</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>242</v>
+      </c>
+      <c r="C115" s="1">
+        <v>39007</v>
+      </c>
+      <c r="D115" t="s">
+        <v>194</v>
+      </c>
+      <c r="E115" t="s">
+        <v>227</v>
+      </c>
+      <c r="F115" t="s">
+        <v>24</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>243</v>
+      </c>
+      <c r="C116" s="1">
+        <v>39028</v>
+      </c>
+      <c r="D116" t="s">
+        <v>44</v>
+      </c>
+      <c r="E116" t="s">
+        <v>144</v>
+      </c>
+      <c r="F116" t="s">
+        <v>24</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>244</v>
+      </c>
+      <c r="C117" s="1">
+        <v>39870</v>
+      </c>
+      <c r="D117" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" t="s">
+        <v>245</v>
+      </c>
+      <c r="F117" t="s">
+        <v>24</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>246</v>
+      </c>
+      <c r="C118" s="1">
+        <v>38678</v>
+      </c>
+      <c r="D118" t="s">
+        <v>44</v>
+      </c>
+      <c r="E118" t="s">
+        <v>119</v>
+      </c>
+      <c r="F118" t="s">
+        <v>24</v>
+      </c>
+      <c r="G118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>247</v>
+      </c>
+      <c r="C119" s="1">
+        <v>38909</v>
+      </c>
+      <c r="D119" t="s">
+        <v>44</v>
+      </c>
+      <c r="E119" t="s">
+        <v>248</v>
+      </c>
+      <c r="F119" t="s">
+        <v>24</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>249</v>
+      </c>
+      <c r="C120" s="1">
+        <v>38663</v>
+      </c>
+      <c r="D120" t="s">
+        <v>43</v>
+      </c>
+      <c r="E120" t="s">
+        <v>119</v>
+      </c>
+      <c r="F120" t="s">
+        <v>24</v>
+      </c>
+      <c r="G120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>250</v>
+      </c>
+      <c r="C121" s="1">
+        <v>38468</v>
+      </c>
+      <c r="D121" t="s">
+        <v>48</v>
+      </c>
+      <c r="E121" t="s">
+        <v>251</v>
+      </c>
+      <c r="F121" t="s">
+        <v>24</v>
+      </c>
+      <c r="G121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>252</v>
+      </c>
+      <c r="C122" s="1">
+        <v>40078</v>
+      </c>
+      <c r="D122" t="s">
+        <v>44</v>
+      </c>
+      <c r="E122" t="s">
+        <v>62</v>
+      </c>
+      <c r="F122" t="s">
+        <v>24</v>
+      </c>
+      <c r="G122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>253</v>
+      </c>
+      <c r="C123" s="1">
+        <v>38671</v>
+      </c>
+      <c r="D123" t="s">
+        <v>43</v>
+      </c>
+      <c r="E123" t="s">
+        <v>254</v>
+      </c>
+      <c r="F123" t="s">
+        <v>24</v>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>255</v>
+      </c>
+      <c r="C124" s="1">
+        <v>39855</v>
+      </c>
+      <c r="D124" t="s">
+        <v>48</v>
+      </c>
+      <c r="E124" t="s">
+        <v>107</v>
+      </c>
+      <c r="F124" t="s">
+        <v>24</v>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C125" s="1">
+        <v>39402</v>
+      </c>
+      <c r="D125" t="s">
+        <v>45</v>
+      </c>
+      <c r="E125" t="s">
+        <v>138</v>
+      </c>
+      <c r="F125" t="s">
+        <v>24</v>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>257</v>
+      </c>
+      <c r="C126" s="1">
+        <v>39518</v>
+      </c>
+      <c r="D126" t="s">
+        <v>43</v>
+      </c>
+      <c r="E126" t="s">
+        <v>254</v>
+      </c>
+      <c r="F126" t="s">
+        <v>24</v>
+      </c>
+      <c r="G126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>258</v>
+      </c>
+      <c r="C127" s="1">
+        <v>38642</v>
+      </c>
+      <c r="D127" t="s">
+        <v>44</v>
+      </c>
+      <c r="E127" t="s">
+        <v>254</v>
+      </c>
+      <c r="F127" t="s">
+        <v>24</v>
+      </c>
+      <c r="G127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>259</v>
+      </c>
+      <c r="C128" s="1">
+        <v>39365</v>
+      </c>
+      <c r="D128" t="s">
+        <v>44</v>
+      </c>
+      <c r="E128" t="s">
+        <v>260</v>
+      </c>
+      <c r="F128" t="s">
+        <v>24</v>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>261</v>
+      </c>
+      <c r="C129" s="1">
+        <v>39365</v>
+      </c>
+      <c r="D129" t="s">
+        <v>44</v>
+      </c>
+      <c r="E129" t="s">
+        <v>260</v>
+      </c>
+      <c r="F129" t="s">
+        <v>24</v>
+      </c>
+      <c r="G129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>262</v>
+      </c>
+      <c r="C130" s="1">
+        <v>39366</v>
+      </c>
+      <c r="D130" t="s">
+        <v>42</v>
+      </c>
+      <c r="E130" t="s">
+        <v>260</v>
+      </c>
+      <c r="F130" t="s">
+        <v>24</v>
+      </c>
+      <c r="G130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>263</v>
+      </c>
+      <c r="C131" s="1">
+        <v>39258</v>
+      </c>
+      <c r="D131" t="s">
+        <v>44</v>
+      </c>
+      <c r="E131" t="s">
+        <v>264</v>
+      </c>
+      <c r="F131" t="s">
+        <v>24</v>
+      </c>
+      <c r="G131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>265</v>
+      </c>
+      <c r="C132" s="1">
+        <v>38860</v>
+      </c>
+      <c r="D132" t="s">
+        <v>46</v>
+      </c>
+      <c r="E132" t="s">
+        <v>266</v>
+      </c>
+      <c r="F132" t="s">
+        <v>24</v>
+      </c>
+      <c r="G132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>267</v>
+      </c>
+      <c r="C133" s="1">
+        <v>38910</v>
+      </c>
+      <c r="D133" t="s">
+        <v>48</v>
+      </c>
+      <c r="E133" t="s">
+        <v>268</v>
+      </c>
+      <c r="F133" t="s">
+        <v>24</v>
+      </c>
+      <c r="G133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>269</v>
+      </c>
+      <c r="C134" s="1">
+        <v>40862</v>
+      </c>
+      <c r="D134" t="s">
+        <v>44</v>
+      </c>
+      <c r="E134" t="s">
+        <v>270</v>
+      </c>
+      <c r="F134" t="s">
+        <v>24</v>
+      </c>
+      <c r="G134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="C135" s="1">
+        <v>40435</v>
+      </c>
+      <c r="D135" t="s">
+        <v>44</v>
+      </c>
+      <c r="E135" t="s">
+        <v>62</v>
+      </c>
+      <c r="F135" t="s">
+        <v>24</v>
+      </c>
+      <c r="G135" t="b">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>272</v>
+      </c>
+      <c r="C136" s="1">
+        <v>39658</v>
+      </c>
+      <c r="D136" t="s">
+        <v>48</v>
+      </c>
+      <c r="E136" t="s">
+        <v>177</v>
+      </c>
+      <c r="F136" t="s">
+        <v>24</v>
+      </c>
+      <c r="G136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>273</v>
+      </c>
+      <c r="C137" s="1">
+        <v>36976</v>
+      </c>
+      <c r="D137" t="s">
+        <v>44</v>
+      </c>
+      <c r="E137" t="s">
+        <v>274</v>
+      </c>
+      <c r="F137" t="s">
+        <v>24</v>
+      </c>
+      <c r="G137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>275</v>
+      </c>
+      <c r="C138" s="1">
+        <v>41219</v>
+      </c>
+      <c r="D138" t="s">
+        <v>44</v>
+      </c>
+      <c r="E138" t="s">
+        <v>270</v>
+      </c>
+      <c r="F138" t="s">
+        <v>24</v>
+      </c>
+      <c r="G138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>276</v>
+      </c>
+      <c r="C139" s="1">
+        <v>40967</v>
+      </c>
+      <c r="D139" t="s">
+        <v>48</v>
+      </c>
+      <c r="E139" t="s">
+        <v>277</v>
+      </c>
+      <c r="F139" t="s">
+        <v>24</v>
+      </c>
+      <c r="G139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>278</v>
+      </c>
+      <c r="C140" s="1">
+        <v>40486</v>
+      </c>
+      <c r="D140" t="s">
+        <v>46</v>
+      </c>
+      <c r="E140" t="s">
+        <v>279</v>
+      </c>
+      <c r="F140" t="s">
+        <v>24</v>
+      </c>
+      <c r="G140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>280</v>
+      </c>
+      <c r="C141" s="1">
+        <v>40939</v>
+      </c>
+      <c r="D141" t="s">
+        <v>48</v>
+      </c>
+      <c r="E141" t="s">
+        <v>177</v>
+      </c>
+      <c r="F141" t="s">
+        <v>24</v>
+      </c>
+      <c r="G141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>281</v>
+      </c>
+      <c r="C142" s="1">
+        <v>39759</v>
+      </c>
+      <c r="D142" t="s">
+        <v>44</v>
+      </c>
+      <c r="E142" t="s">
+        <v>144</v>
+      </c>
+      <c r="F142" t="s">
+        <v>24</v>
+      </c>
+      <c r="G142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>282</v>
+      </c>
+      <c r="C143" s="1">
+        <v>39910</v>
+      </c>
+      <c r="D143" t="s">
+        <v>43</v>
+      </c>
+      <c r="E143" t="s">
+        <v>264</v>
+      </c>
+      <c r="F143" t="s">
+        <v>24</v>
+      </c>
+      <c r="G143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>283</v>
+      </c>
+      <c r="C144" s="1">
+        <v>39555</v>
+      </c>
+      <c r="D144" t="s">
+        <v>48</v>
+      </c>
+      <c r="E144" t="s">
+        <v>18</v>
+      </c>
+      <c r="F144" t="s">
+        <v>24</v>
+      </c>
+      <c r="G144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>284</v>
+      </c>
+      <c r="C145" s="1">
+        <v>38678</v>
+      </c>
+      <c r="D145" t="s">
+        <v>47</v>
+      </c>
+      <c r="E145" t="s">
+        <v>285</v>
+      </c>
+      <c r="F145" t="s">
+        <v>24</v>
+      </c>
+      <c r="G145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>287</v>
+      </c>
+      <c r="C146" s="1">
+        <v>36498</v>
+      </c>
+      <c r="D146" t="s">
+        <v>48</v>
+      </c>
+      <c r="E146" t="s">
+        <v>18</v>
+      </c>
+      <c r="F146" t="s">
+        <v>17</v>
+      </c>
+      <c r="G146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>288</v>
+      </c>
+      <c r="C147" s="1">
+        <v>36494</v>
+      </c>
+      <c r="D147" t="s">
+        <v>48</v>
+      </c>
+      <c r="E147" t="s">
+        <v>18</v>
+      </c>
+      <c r="F147" t="s">
+        <v>17</v>
+      </c>
+      <c r="G147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>289</v>
+      </c>
+      <c r="C148" s="1">
+        <v>36372</v>
+      </c>
+      <c r="D148" t="s">
+        <v>42</v>
+      </c>
+      <c r="E148" t="s">
+        <v>221</v>
+      </c>
+      <c r="F148" t="s">
+        <v>17</v>
+      </c>
+      <c r="G148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>290</v>
+      </c>
+      <c r="C149" s="1">
+        <v>36372</v>
+      </c>
+      <c r="D149" t="s">
+        <v>46</v>
+      </c>
+      <c r="E149" t="s">
+        <v>291</v>
+      </c>
+      <c r="F149" t="s">
+        <v>17</v>
+      </c>
+      <c r="G149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <f t="shared" ref="A150:A168" si="3">A149+1</f>
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>292</v>
+      </c>
+      <c r="C150" s="1">
+        <v>36280</v>
+      </c>
+      <c r="D150" t="s">
+        <v>48</v>
+      </c>
+      <c r="E150" t="s">
+        <v>18</v>
+      </c>
+      <c r="F150" t="s">
+        <v>17</v>
+      </c>
+      <c r="G150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>293</v>
+      </c>
+      <c r="C151" s="1">
+        <v>36307</v>
+      </c>
+      <c r="D151" t="s">
+        <v>44</v>
+      </c>
+      <c r="E151" t="s">
+        <v>294</v>
+      </c>
+      <c r="F151" t="s">
+        <v>17</v>
+      </c>
+      <c r="G151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <f t="shared" si="3"/>
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>295</v>
+      </c>
+      <c r="C152" s="1">
+        <v>36280</v>
+      </c>
+      <c r="D152" t="s">
+        <v>48</v>
+      </c>
+      <c r="E152" t="s">
+        <v>291</v>
+      </c>
+      <c r="F152" t="s">
+        <v>17</v>
+      </c>
+      <c r="G152" t="b">
+        <v>1</v>
+      </c>
+      <c r="H152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <f t="shared" si="3"/>
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>296</v>
+      </c>
+      <c r="C153" s="1">
+        <v>36292</v>
+      </c>
+      <c r="D153" t="s">
+        <v>48</v>
+      </c>
+      <c r="E153" t="s">
+        <v>298</v>
+      </c>
+      <c r="F153" t="s">
+        <v>17</v>
+      </c>
+      <c r="G153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>297</v>
+      </c>
+      <c r="C154" s="1">
+        <v>35769</v>
+      </c>
+      <c r="D154" t="s">
+        <v>48</v>
+      </c>
+      <c r="E154" t="s">
+        <v>18</v>
+      </c>
+      <c r="F154" t="s">
+        <v>17</v>
+      </c>
+      <c r="G154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>299</v>
+      </c>
+      <c r="C155" s="1">
+        <v>36265</v>
+      </c>
+      <c r="D155" t="s">
+        <v>45</v>
+      </c>
+      <c r="E155" t="s">
+        <v>298</v>
+      </c>
+      <c r="F155" t="s">
+        <v>17</v>
+      </c>
+      <c r="G155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <f t="shared" si="3"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <f t="shared" si="3"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <f t="shared" si="3"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <f t="shared" si="3"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <f t="shared" si="3"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <f t="shared" si="3"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <f t="shared" si="3"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <f t="shared" si="3"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <f t="shared" si="3"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <f t="shared" si="3"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <f t="shared" si="3"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <f t="shared" si="3"/>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3248,10 +5369,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B0A4AE-C2F8-404D-A551-5227A91C7005}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3362,6 +5483,17 @@
       </c>
       <c r="C9" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Wii and GBA games
</commit_message>
<xml_diff>
--- a/Video Games.xlsx
+++ b/Video Games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Video-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB23BBA-BC82-4EC3-888D-B29F72F2030D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C766A23C-B2ED-4B7D-BCCE-0EACEB28B536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="335">
   <si>
     <t>Name</t>
   </si>
@@ -937,6 +937,111 @@
   </si>
   <si>
     <t>Biomotor Unitron</t>
+  </si>
+  <si>
+    <t>Digital Eclipse</t>
+  </si>
+  <si>
+    <t>Disney's Lilo &amp; Stitch</t>
+  </si>
+  <si>
+    <t>Quad Desert Fury</t>
+  </si>
+  <si>
+    <t>Skyworks Interactive Inc</t>
+  </si>
+  <si>
+    <t>Frogger's Adventure Temple of the Frog</t>
+  </si>
+  <si>
+    <t>Konami Software Shanghai</t>
+  </si>
+  <si>
+    <t>Konami Collector's Series Arcade Advanced</t>
+  </si>
+  <si>
+    <t>Dragon Ball Z Legacy of Goku</t>
+  </si>
+  <si>
+    <t>Webfoot Technologies</t>
+  </si>
+  <si>
+    <t>Lego Star Wars The Video Game</t>
+  </si>
+  <si>
+    <t>The Spongebob Squarepants Movie</t>
+  </si>
+  <si>
+    <t>Heavy Iron Studios</t>
+  </si>
+  <si>
+    <t>Disney's Tarzan Return to the Jungle</t>
+  </si>
+  <si>
+    <t>Savage Entertainment</t>
+  </si>
+  <si>
+    <t>He-Man Power of Grayskull</t>
+  </si>
+  <si>
+    <t>The Wild Thornberrys Movie</t>
+  </si>
+  <si>
+    <t>Human Soft</t>
+  </si>
+  <si>
+    <t>Classic NES Series Ice Climber</t>
+  </si>
+  <si>
+    <t>Men in Black The Series</t>
+  </si>
+  <si>
+    <t>David A Palmer Productions</t>
+  </si>
+  <si>
+    <t>Naruto Clash of Ninja Revolution</t>
+  </si>
+  <si>
+    <t>Tomy</t>
+  </si>
+  <si>
+    <t>Sonic Colors</t>
+  </si>
+  <si>
+    <t>Sonic Team</t>
+  </si>
+  <si>
+    <t>Speed Racer The Videogame</t>
+  </si>
+  <si>
+    <t>Sidhe Interactive</t>
+  </si>
+  <si>
+    <t>Wii Fit</t>
+  </si>
+  <si>
+    <t>Nintendo EAD Group No 5</t>
+  </si>
+  <si>
+    <t>Wii Play</t>
+  </si>
+  <si>
+    <t>Mario Kart Wii</t>
+  </si>
+  <si>
+    <t>Super Smash Bros Brawl</t>
+  </si>
+  <si>
+    <t>Battalion Wars 2</t>
+  </si>
+  <si>
+    <t>Kuju Entertainment</t>
+  </si>
+  <si>
+    <t>Donkey Kong Country Returns</t>
+  </si>
+  <si>
+    <t>Retro Studios</t>
   </si>
 </sst>
 </file>
@@ -1295,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58CEA45-1A97-47FC-8ACE-673891E6166E}">
-  <dimension ref="A1:H168"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4902,7 +5007,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150">
-        <f t="shared" ref="A150:A168" si="3">A149+1</f>
+        <f t="shared" ref="A150:A177" si="3">A149+1</f>
         <v>149</v>
       </c>
       <c r="B150" t="s">
@@ -5052,77 +5157,506 @@
         <f t="shared" si="3"/>
         <v>155</v>
       </c>
+      <c r="B156" t="s">
+        <v>301</v>
+      </c>
+      <c r="C156" s="1">
+        <v>37414</v>
+      </c>
+      <c r="D156" t="s">
+        <v>43</v>
+      </c>
+      <c r="E156" t="s">
+        <v>300</v>
+      </c>
+      <c r="F156" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157">
         <f t="shared" si="3"/>
         <v>156</v>
       </c>
+      <c r="B157" t="s">
+        <v>302</v>
+      </c>
+      <c r="C157" s="1">
+        <v>37677</v>
+      </c>
+      <c r="D157" t="s">
+        <v>47</v>
+      </c>
+      <c r="E157" t="s">
+        <v>303</v>
+      </c>
+      <c r="F157" t="s">
+        <v>13</v>
+      </c>
+      <c r="G157" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158">
         <f t="shared" si="3"/>
         <v>157</v>
       </c>
+      <c r="B158" t="s">
+        <v>304</v>
+      </c>
+      <c r="C158" s="1">
+        <v>37216</v>
+      </c>
+      <c r="D158" t="s">
+        <v>43</v>
+      </c>
+      <c r="E158" t="s">
+        <v>305</v>
+      </c>
+      <c r="F158" t="s">
+        <v>13</v>
+      </c>
+      <c r="G158" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159">
         <f t="shared" si="3"/>
         <v>158</v>
       </c>
+      <c r="B159" t="s">
+        <v>306</v>
+      </c>
+      <c r="C159" s="1">
+        <v>37337</v>
+      </c>
+      <c r="E159" t="s">
+        <v>166</v>
+      </c>
+      <c r="F159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G159" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160">
         <f t="shared" si="3"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B160" t="s">
+        <v>307</v>
+      </c>
+      <c r="C160" s="1">
+        <v>37390</v>
+      </c>
+      <c r="D160" t="s">
+        <v>45</v>
+      </c>
+      <c r="E160" t="s">
+        <v>308</v>
+      </c>
+      <c r="F160" t="s">
+        <v>13</v>
+      </c>
+      <c r="G160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B161" t="s">
+        <v>309</v>
+      </c>
+      <c r="C161" s="1">
+        <v>38440</v>
+      </c>
+      <c r="D161" t="s">
+        <v>43</v>
+      </c>
+      <c r="E161" t="s">
+        <v>116</v>
+      </c>
+      <c r="F161" t="s">
+        <v>13</v>
+      </c>
+      <c r="G161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162">
         <f t="shared" si="3"/>
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B162" t="s">
+        <v>310</v>
+      </c>
+      <c r="C162" s="1">
+        <v>38287</v>
+      </c>
+      <c r="D162" t="s">
+        <v>43</v>
+      </c>
+      <c r="E162" t="s">
+        <v>311</v>
+      </c>
+      <c r="F162" t="s">
+        <v>13</v>
+      </c>
+      <c r="G162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163">
         <f t="shared" si="3"/>
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B163" t="s">
+        <v>312</v>
+      </c>
+      <c r="C163" s="1">
+        <v>37513</v>
+      </c>
+      <c r="D163" t="s">
+        <v>43</v>
+      </c>
+      <c r="E163" t="s">
+        <v>300</v>
+      </c>
+      <c r="F163" t="s">
+        <v>13</v>
+      </c>
+      <c r="G163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164">
         <f t="shared" si="3"/>
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B164" t="s">
+        <v>314</v>
+      </c>
+      <c r="C164" s="1">
+        <v>37558</v>
+      </c>
+      <c r="D164" t="s">
+        <v>43</v>
+      </c>
+      <c r="E164" t="s">
+        <v>313</v>
+      </c>
+      <c r="F164" t="s">
+        <v>13</v>
+      </c>
+      <c r="G164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165">
         <f t="shared" si="3"/>
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B165" t="s">
+        <v>315</v>
+      </c>
+      <c r="C165" s="1">
+        <v>37573</v>
+      </c>
+      <c r="D165" t="s">
+        <v>43</v>
+      </c>
+      <c r="E165" t="s">
+        <v>316</v>
+      </c>
+      <c r="F165" t="s">
+        <v>13</v>
+      </c>
+      <c r="G165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166">
         <f t="shared" si="3"/>
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B166" t="s">
+        <v>317</v>
+      </c>
+      <c r="C166" s="1">
+        <v>38140</v>
+      </c>
+      <c r="D166" t="s">
+        <v>43</v>
+      </c>
+      <c r="E166" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" t="s">
+        <v>13</v>
+      </c>
+      <c r="G166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167">
         <f t="shared" si="3"/>
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B167" t="s">
+        <v>318</v>
+      </c>
+      <c r="C167" s="1">
+        <v>37145</v>
+      </c>
+      <c r="D167" t="s">
+        <v>43</v>
+      </c>
+      <c r="E167" t="s">
+        <v>319</v>
+      </c>
+      <c r="F167" t="s">
+        <v>13</v>
+      </c>
+      <c r="G167" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168">
         <f t="shared" si="3"/>
         <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>320</v>
+      </c>
+      <c r="C168" s="1">
+        <v>39135</v>
+      </c>
+      <c r="D168" t="s">
+        <v>48</v>
+      </c>
+      <c r="E168" t="s">
+        <v>321</v>
+      </c>
+      <c r="F168" t="s">
+        <v>10</v>
+      </c>
+      <c r="G168" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>322</v>
+      </c>
+      <c r="C169" s="1">
+        <v>40493</v>
+      </c>
+      <c r="D169" t="s">
+        <v>43</v>
+      </c>
+      <c r="E169" t="s">
+        <v>323</v>
+      </c>
+      <c r="F169" t="s">
+        <v>10</v>
+      </c>
+      <c r="G169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>324</v>
+      </c>
+      <c r="C170" s="1">
+        <v>39574</v>
+      </c>
+      <c r="D170" t="s">
+        <v>47</v>
+      </c>
+      <c r="E170" t="s">
+        <v>325</v>
+      </c>
+      <c r="F170" t="s">
+        <v>10</v>
+      </c>
+      <c r="G170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <f t="shared" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>326</v>
+      </c>
+      <c r="C171" s="1">
+        <v>39589</v>
+      </c>
+      <c r="E171" t="s">
+        <v>327</v>
+      </c>
+      <c r="F171" t="s">
+        <v>10</v>
+      </c>
+      <c r="G171" t="b">
+        <v>1</v>
+      </c>
+      <c r="H171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <f t="shared" si="3"/>
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>328</v>
+      </c>
+      <c r="C172" s="1">
+        <v>39057</v>
+      </c>
+      <c r="D172" t="s">
+        <v>43</v>
+      </c>
+      <c r="E172" t="s">
+        <v>11</v>
+      </c>
+      <c r="F172" t="s">
+        <v>10</v>
+      </c>
+      <c r="G172" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <f t="shared" si="3"/>
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>329</v>
+      </c>
+      <c r="C173" s="1">
+        <v>39548</v>
+      </c>
+      <c r="D173" t="s">
+        <v>47</v>
+      </c>
+      <c r="E173" t="s">
+        <v>11</v>
+      </c>
+      <c r="F173" t="s">
+        <v>10</v>
+      </c>
+      <c r="G173" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <f t="shared" si="3"/>
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>330</v>
+      </c>
+      <c r="C174" s="1">
+        <v>39478</v>
+      </c>
+      <c r="D174" t="s">
+        <v>48</v>
+      </c>
+      <c r="E174" t="s">
+        <v>11</v>
+      </c>
+      <c r="F174" t="s">
+        <v>10</v>
+      </c>
+      <c r="G174" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <f t="shared" si="3"/>
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>331</v>
+      </c>
+      <c r="C175" s="1">
+        <v>39384</v>
+      </c>
+      <c r="D175" t="s">
+        <v>42</v>
+      </c>
+      <c r="E175" t="s">
+        <v>332</v>
+      </c>
+      <c r="F175" t="s">
+        <v>10</v>
+      </c>
+      <c r="G175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <f t="shared" si="3"/>
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>333</v>
+      </c>
+      <c r="C176" s="1">
+        <v>40503</v>
+      </c>
+      <c r="D176" t="s">
+        <v>43</v>
+      </c>
+      <c r="E176" t="s">
+        <v>334</v>
+      </c>
+      <c r="F176" t="s">
+        <v>10</v>
+      </c>
+      <c r="G176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <f t="shared" si="3"/>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to developer worksheet. Reading excel sheets into notebook
</commit_message>
<xml_diff>
--- a/Video Games.xlsx
+++ b/Video Games.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Video-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5A26E5-5319-420C-B335-02A31B29BBA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAEE603-74AD-44E3-8FA9-D12026A1C440}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
   </bookViews>
   <sheets>
-    <sheet name="VideoGames" sheetId="1" r:id="rId1"/>
-    <sheet name="Consoles" sheetId="2" r:id="rId2"/>
-    <sheet name="Genres" sheetId="3" r:id="rId3"/>
-    <sheet name="Developers" sheetId="4" r:id="rId4"/>
-    <sheet name="Publishers" sheetId="5" r:id="rId5"/>
+    <sheet name="video_games" sheetId="1" r:id="rId1"/>
+    <sheet name="genres" sheetId="3" r:id="rId2"/>
+    <sheet name="consoles" sheetId="2" r:id="rId3"/>
+    <sheet name="developers" sheetId="4" r:id="rId4"/>
+    <sheet name="publishers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="724">
   <si>
     <t>Name</t>
   </si>
@@ -2074,6 +2074,141 @@
   </si>
   <si>
     <t>DeveloperID</t>
+  </si>
+  <si>
+    <t>Roswell, Georgia, U.S.</t>
+  </si>
+  <si>
+    <t>Amsterdam, Netherlands</t>
+  </si>
+  <si>
+    <t>Bellevue, Washington, U.S.</t>
+  </si>
+  <si>
+    <t>Malmö, Sweden</t>
+  </si>
+  <si>
+    <t>Santa Monica, California, US</t>
+  </si>
+  <si>
+    <t>Woodland Hills, California, United States</t>
+  </si>
+  <si>
+    <t>Foster City, California, United States</t>
+  </si>
+  <si>
+    <t>Stockholm, Sweden</t>
+  </si>
+  <si>
+    <t>Fukuoka, Japan</t>
+  </si>
+  <si>
+    <t>Montreal, Canada</t>
+  </si>
+  <si>
+    <t>Burbank, California, US</t>
+  </si>
+  <si>
+    <t>Irvine, California, U.S.</t>
+  </si>
+  <si>
+    <t>Maidenhead, England</t>
+  </si>
+  <si>
+    <t>Knutsford, England</t>
+  </si>
+  <si>
+    <t>Cary, North Carolina, US</t>
+  </si>
+  <si>
+    <t>Burnaby, British Columbia, Canada</t>
+  </si>
+  <si>
+    <t>Frisco, Texas, U.S.</t>
+  </si>
+  <si>
+    <t>Castelnau-le-Lez, France</t>
+  </si>
+  <si>
+    <t>Brighton, United Kingdom</t>
+  </si>
+  <si>
+    <t>Salt Lake City, Utah, USA</t>
+  </si>
+  <si>
+    <t>Chūō-ku, Osaka, Japan</t>
+  </si>
+  <si>
+    <t>Los Angeles, US</t>
+  </si>
+  <si>
+    <t>Twycross, Leicestershire, England</t>
+  </si>
+  <si>
+    <t>Berlin, Germany</t>
+  </si>
+  <si>
+    <t>Maitland, Florida</t>
+  </si>
+  <si>
+    <t>Berkeley, California, United States</t>
+  </si>
+  <si>
+    <t>Bristol, England, UK</t>
+  </si>
+  <si>
+    <t>San Francisco, CA, USA</t>
+  </si>
+  <si>
+    <t>Austin, Texas, U.S.</t>
+  </si>
+  <si>
+    <t>Edmonton, Alberta, Canada</t>
+  </si>
+  <si>
+    <t>Yokohama, Japan</t>
+  </si>
+  <si>
+    <t>Suita, Osaka Prefecture, Japan</t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Newport Beach, California, US</t>
+  </si>
+  <si>
+    <t>Redmond, Washington, US</t>
+  </si>
+  <si>
+    <t>Ginza, Chūō, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>San Francisco, California, United States</t>
+  </si>
+  <si>
+    <t>Shinagawa, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Sheffield, England</t>
+  </si>
+  <si>
+    <t>Warrington, Cheshire, United Kingdom</t>
+  </si>
+  <si>
+    <t>Chicago, Illinois</t>
+  </si>
+  <si>
+    <t>Emeryville, California, US</t>
+  </si>
+  <si>
+    <t>Hoffman Estates, Illinois, US</t>
+  </si>
+  <si>
+    <t>Ōta, Tokyo, Japan</t>
   </si>
 </sst>
 </file>
@@ -2115,12 +2250,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2437,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58CEA45-1A97-47FC-8ACE-673891E6166E}">
   <dimension ref="A1:I410"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B78" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14430,6 +14567,173 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B0A4AE-C2F8-404D-A551-5227A91C7005}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="60.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" ref="A4:A7" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C11" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>674</v>
+      </c>
+      <c r="C12" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>676</v>
+      </c>
+      <c r="C13" t="s">
+        <v>677</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504D8DBC-C745-4910-814D-6E09B0045555}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -14700,187 +15004,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B0A4AE-C2F8-404D-A551-5227A91C7005}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="60.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <f t="shared" ref="A4:A7" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>571</v>
-      </c>
-      <c r="C11" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>674</v>
-      </c>
-      <c r="C12" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>676</v>
-      </c>
-      <c r="C13" t="s">
-        <v>677</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85547471-D81A-4F7D-B243-B5E5EB852E1E}">
   <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.08984375" customWidth="1"/>
     <col min="2" max="2" width="37.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -14893,7 +15030,7 @@
       <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -14903,6 +15040,12 @@
       </c>
       <c r="B2" t="s">
         <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>679</v>
+      </c>
+      <c r="D2" s="1">
+        <v>38400</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -14912,550 +15055,874 @@
       <c r="B3" t="s">
         <v>58</v>
       </c>
+      <c r="C3" t="s">
+        <v>680</v>
+      </c>
+      <c r="D3" s="1">
+        <v>36526</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" ref="A4:A35" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
       </c>
+      <c r="C4" t="s">
+        <v>681</v>
+      </c>
+      <c r="D4" s="1">
+        <v>33359</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
       </c>
+      <c r="C5" t="s">
+        <v>682</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1997</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
+      <c r="C6" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" s="1">
+        <v>30952</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>65</v>
       </c>
+      <c r="C7" t="s">
+        <v>684</v>
+      </c>
+      <c r="D7" s="1">
+        <v>37377</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>66</v>
       </c>
+      <c r="C8" t="s">
+        <v>685</v>
+      </c>
+      <c r="D8" s="1">
+        <v>40015</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>98</v>
       </c>
+      <c r="C9" t="s">
+        <v>686</v>
+      </c>
+      <c r="D9" s="1">
+        <v>33725</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
       </c>
+      <c r="C10" t="s">
+        <v>687</v>
+      </c>
+      <c r="D10" s="1">
+        <v>35111</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>69</v>
       </c>
+      <c r="C11" t="s">
+        <v>683</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1996</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>71</v>
       </c>
+      <c r="C12" t="s">
+        <v>688</v>
+      </c>
+      <c r="D12" s="1">
+        <v>35545</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>73</v>
       </c>
+      <c r="C13" t="s">
+        <v>689</v>
+      </c>
+      <c r="D13" s="1">
+        <v>34393</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
+      <c r="C14" t="s">
+        <v>690</v>
+      </c>
+      <c r="D14" s="1">
+        <v>33270</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>76</v>
       </c>
+      <c r="C15" t="s">
+        <v>691</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2005</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>692</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>693</v>
+      </c>
+      <c r="D17" s="1">
+        <v>35382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>694</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>695</v>
+      </c>
+      <c r="D19" s="1">
+        <v>36207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>696</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>697</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>698</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>699</v>
+      </c>
+      <c r="D23" s="1">
+        <v>29005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>700</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>701</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>702</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>703</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>704</v>
+      </c>
+      <c r="D28" s="1">
+        <v>34578</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>705</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>706</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>707</v>
+      </c>
+      <c r="D31" s="1">
+        <v>35384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>708</v>
+      </c>
+      <c r="D32" s="1">
+        <v>34731</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
-        <f>A33+1</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>709</v>
+      </c>
+      <c r="D34" s="1">
+        <v>39904</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
-        <f>A34+1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>693</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
-        <f>A35+1</f>
+        <f t="shared" ref="A36:A67" si="1">A35+1</f>
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>710</v>
+      </c>
+      <c r="D36" s="1">
+        <v>28693</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
-        <f>A36+1</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>711</v>
+      </c>
+      <c r="D37" s="1">
+        <v>31717</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
-        <f>A37+1</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>712</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
-        <f>A38+1</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>712</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
-        <f>A39+1</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>713</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
-        <f>A40+1</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>714</v>
+      </c>
+      <c r="D41" s="1">
+        <v>36586</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
-        <f>A41+1</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>715</v>
+      </c>
+      <c r="D42" s="1">
+        <v>25283</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
-        <f>A42+1</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>716</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
-        <f>A43+1</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>717</v>
+      </c>
+      <c r="D44" s="1">
+        <v>34043</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
-        <f>A44+1</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>709</v>
+      </c>
+      <c r="D45" s="1">
+        <v>32275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
-        <f>A45+1</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>717</v>
+      </c>
+      <c r="D46" s="1">
+        <v>35004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
-        <f>A46+1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
-        <f>A47+1</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>699</v>
+      </c>
+      <c r="D48" s="1">
+        <v>29005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
-        <f>A48+1</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>707</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
-        <f>A49+1</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
-        <f>A50+1</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="D51" s="1">
+        <v>36637</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
-        <f>A51+1</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>718</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
-        <f>A52+1</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>719</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
-        <f>A53+1</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>711</v>
+      </c>
+      <c r="D54" s="1">
+        <v>37575</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
-        <f>A54+1</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>720</v>
+      </c>
+      <c r="D55" s="1">
+        <v>35467</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
-        <f>A55+1</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>717</v>
+      </c>
+      <c r="D56" s="1">
+        <v>22070</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
-        <f>A56+1</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>721</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
-        <f>A57+1</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
+        <v>722</v>
+      </c>
+      <c r="D58" s="1">
+        <v>34060</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
-        <f>A58+1</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>723</v>
+      </c>
+      <c r="D59" s="1">
+        <v>20241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
-        <f>A59+1</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
-        <f>A60+1</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
-        <f>A61+1</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
-        <f>A62+1</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
-        <f>A63+1</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
@@ -15464,7 +15931,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
-        <f>A64+1</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B65" t="s">
@@ -15473,7 +15940,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
-        <f>A65+1</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="B66" t="s">
@@ -15482,7 +15949,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
-        <f>A66+1</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="B67" t="s">
@@ -15491,7 +15958,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
-        <f>A67+1</f>
+        <f t="shared" ref="A68:A99" si="2">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" t="s">
@@ -15500,7 +15967,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
-        <f>A68+1</f>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -15509,7 +15976,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
-        <f>A69+1</f>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B70" t="s">
@@ -15518,7 +15985,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
-        <f>A70+1</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B71" t="s">
@@ -15527,7 +15994,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
-        <f>A71+1</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B72" t="s">
@@ -15536,7 +16003,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
-        <f>A72+1</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="B73" t="s">
@@ -15545,7 +16012,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74">
-        <f>A73+1</f>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="B74" t="s">
@@ -15554,7 +16021,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75">
-        <f>A74+1</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="B75" t="s">
@@ -15563,7 +16030,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
-        <f>A75+1</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B76" t="s">
@@ -15572,7 +16039,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
-        <f>A76+1</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="B77" t="s">
@@ -15581,7 +16048,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78">
-        <f>A77+1</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="B78" t="s">
@@ -15590,7 +16057,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
-        <f>A78+1</f>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B79" t="s">
@@ -15599,7 +16066,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
-        <f>A79+1</f>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="B80" t="s">
@@ -15608,7 +16075,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
-        <f>A80+1</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B81" t="s">
@@ -15617,7 +16084,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
-        <f>A81+1</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B82" t="s">
@@ -15626,7 +16093,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
-        <f>A82+1</f>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B83" t="s">
@@ -15635,7 +16102,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
-        <f>A83+1</f>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -15644,7 +16111,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
-        <f>A84+1</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -15653,7 +16120,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
-        <f>A85+1</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -15662,7 +16129,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
-        <f>A86+1</f>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="B87" t="s">
@@ -15671,7 +16138,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
-        <f>A87+1</f>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -15680,7 +16147,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
-        <f>A88+1</f>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="B89" t="s">
@@ -15689,7 +16156,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
-        <f>A89+1</f>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="B90" t="s">
@@ -15698,7 +16165,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
-        <f>A90+1</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="B91" t="s">
@@ -15707,7 +16174,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
-        <f>A91+1</f>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="B92" t="s">
@@ -15716,7 +16183,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
-        <f>A92+1</f>
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="B93" t="s">
@@ -15725,7 +16192,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
-        <f>A93+1</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="B94" t="s">
@@ -15734,7 +16201,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
-        <f>A94+1</f>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="B95" t="s">
@@ -15743,7 +16210,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
-        <f>A95+1</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="B96" t="s">
@@ -15752,7 +16219,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97">
-        <f>A96+1</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="B97" t="s">
@@ -15761,7 +16228,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98">
-        <f>A97+1</f>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="B98" t="s">
@@ -15770,7 +16237,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99">
-        <f>A98+1</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="B99" t="s">
@@ -15779,7 +16246,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100">
-        <f>A99+1</f>
+        <f t="shared" ref="A100:A131" si="3">A99+1</f>
         <v>99</v>
       </c>
       <c r="B100" t="s">
@@ -15788,7 +16255,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101">
-        <f>A100+1</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="B101" t="s">
@@ -15797,7 +16264,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102">
-        <f>A101+1</f>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="B102" t="s">
@@ -15806,7 +16273,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103">
-        <f>A102+1</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="B103" t="s">
@@ -15815,7 +16282,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104">
-        <f>A103+1</f>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="B104" t="s">
@@ -15824,7 +16291,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105">
-        <f>A104+1</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="B105" t="s">
@@ -15833,7 +16300,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106">
-        <f>A105+1</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="B106" t="s">
@@ -15842,7 +16309,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107">
-        <f>A106+1</f>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="B107" t="s">
@@ -15851,7 +16318,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108">
-        <f>A107+1</f>
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="B108" t="s">
@@ -15860,7 +16327,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109">
-        <f>A108+1</f>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="B109" t="s">
@@ -15869,7 +16336,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110">
-        <f>A109+1</f>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="B110" t="s">
@@ -15878,7 +16345,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111">
-        <f>A110+1</f>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="B111" t="s">
@@ -15887,7 +16354,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112">
-        <f>A111+1</f>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="B112" t="s">
@@ -15896,7 +16363,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113">
-        <f>A112+1</f>
+        <f t="shared" si="3"/>
         <v>112</v>
       </c>
       <c r="B113" t="s">
@@ -15905,7 +16372,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114">
-        <f>A113+1</f>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="B114" t="s">
@@ -15914,7 +16381,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115">
-        <f>A114+1</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="B115" t="s">
@@ -15923,7 +16390,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116">
-        <f>A115+1</f>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="B116" t="s">
@@ -15932,7 +16399,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117">
-        <f>A116+1</f>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="B117" t="s">
@@ -15941,7 +16408,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118">
-        <f>A117+1</f>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="B118" t="s">
@@ -15950,7 +16417,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119">
-        <f>A118+1</f>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="B119" t="s">
@@ -15959,7 +16426,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120">
-        <f>A119+1</f>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="B120" t="s">
@@ -15968,7 +16435,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121">
-        <f>A120+1</f>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="B121" t="s">
@@ -15977,7 +16444,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122">
-        <f>A121+1</f>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="B122" t="s">
@@ -15986,7 +16453,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123">
-        <f>A122+1</f>
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="B123" t="s">
@@ -15995,7 +16462,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124">
-        <f>A123+1</f>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="B124" t="s">
@@ -16004,7 +16471,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125">
-        <f>A124+1</f>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="B125" t="s">
@@ -16013,7 +16480,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126">
-        <f>A125+1</f>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="B126" t="s">
@@ -16022,7 +16489,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127">
-        <f>A126+1</f>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="B127" t="s">
@@ -16031,7 +16498,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128">
-        <f>A127+1</f>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="B128" t="s">
@@ -16040,7 +16507,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129">
-        <f>A128+1</f>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="B129" t="s">
@@ -16049,7 +16516,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130">
-        <f>A129+1</f>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="B130" t="s">
@@ -16058,7 +16525,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131">
-        <f>A130+1</f>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="B131" t="s">
@@ -16067,7 +16534,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132">
-        <f>A131+1</f>
+        <f t="shared" ref="A132:A150" si="4">A131+1</f>
         <v>131</v>
       </c>
       <c r="B132" t="s">
@@ -16076,7 +16543,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133">
-        <f>A132+1</f>
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
       <c r="B133" t="s">
@@ -16085,7 +16552,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134">
-        <f>A133+1</f>
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
       <c r="B134" t="s">
@@ -16094,7 +16561,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135">
-        <f>A134+1</f>
+        <f t="shared" si="4"/>
         <v>134</v>
       </c>
       <c r="B135" t="s">
@@ -16103,7 +16570,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136">
-        <f>A135+1</f>
+        <f t="shared" si="4"/>
         <v>135</v>
       </c>
       <c r="B136" t="s">
@@ -16112,7 +16579,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137">
-        <f>A136+1</f>
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
       <c r="B137" t="s">
@@ -16121,7 +16588,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138">
-        <f>A137+1</f>
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
       <c r="B138" t="s">
@@ -16130,7 +16597,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139">
-        <f>A138+1</f>
+        <f t="shared" si="4"/>
         <v>138</v>
       </c>
       <c r="B139" t="s">
@@ -16139,7 +16606,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140">
-        <f>A139+1</f>
+        <f t="shared" si="4"/>
         <v>139</v>
       </c>
       <c r="B140" t="s">
@@ -16148,7 +16615,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141">
-        <f>A140+1</f>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="B141" t="s">
@@ -16157,7 +16624,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142">
-        <f>A141+1</f>
+        <f t="shared" si="4"/>
         <v>141</v>
       </c>
       <c r="B142" t="s">
@@ -16166,7 +16633,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143">
-        <f>A142+1</f>
+        <f t="shared" si="4"/>
         <v>142</v>
       </c>
       <c r="B143" t="s">
@@ -16175,7 +16642,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144">
-        <f>A143+1</f>
+        <f t="shared" si="4"/>
         <v>143</v>
       </c>
       <c r="B144" t="s">
@@ -16184,7 +16651,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145">
-        <f>A144+1</f>
+        <f t="shared" si="4"/>
         <v>144</v>
       </c>
       <c r="B145" t="s">
@@ -16193,7 +16660,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146">
-        <f>A145+1</f>
+        <f t="shared" si="4"/>
         <v>145</v>
       </c>
       <c r="B146" t="s">
@@ -16202,7 +16669,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147">
-        <f>A146+1</f>
+        <f t="shared" si="4"/>
         <v>146</v>
       </c>
       <c r="B147" t="s">
@@ -16211,7 +16678,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148">
-        <f>A147+1</f>
+        <f t="shared" si="4"/>
         <v>147</v>
       </c>
       <c r="B148" t="s">
@@ -16220,7 +16687,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149">
-        <f>A148+1</f>
+        <f t="shared" si="4"/>
         <v>148</v>
       </c>
       <c r="B149" t="s">
@@ -16229,7 +16696,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150">
-        <f>A149+1</f>
+        <f t="shared" si="4"/>
         <v>149</v>
       </c>
       <c r="B150" t="s">
@@ -16238,7 +16705,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151">
-        <f t="shared" ref="A151:A207" si="0">A150+1</f>
+        <f t="shared" ref="A151:A207" si="5">A150+1</f>
         <v>150</v>
       </c>
       <c r="B151" t="s">
@@ -16247,7 +16714,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
       <c r="B152" t="s">
@@ -16256,7 +16723,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>152</v>
       </c>
       <c r="B153" t="s">
@@ -16265,7 +16732,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
       <c r="B154" t="s">
@@ -16274,7 +16741,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
       <c r="B155" t="s">
@@ -16283,7 +16750,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
       <c r="B156" t="s">
@@ -16292,7 +16759,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>156</v>
       </c>
       <c r="B157" t="s">
@@ -16301,7 +16768,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
       <c r="B158" t="s">
@@ -16310,7 +16777,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>158</v>
       </c>
       <c r="B159" t="s">
@@ -16319,7 +16786,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="B160" t="s">
@@ -16328,7 +16795,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="B161" t="s">
@@ -16337,7 +16804,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="B162" t="s">
@@ -16346,7 +16813,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
       <c r="B163" t="s">
@@ -16355,7 +16822,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
       <c r="B164" t="s">
@@ -16364,7 +16831,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="B165" t="s">
@@ -16373,7 +16840,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="B166" t="s">
@@ -16382,7 +16849,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="B167" t="s">
@@ -16391,13 +16858,13 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="B169" t="s">
@@ -16406,7 +16873,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
       <c r="B170" t="s">
@@ -16415,7 +16882,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="B171" t="s">
@@ -16424,7 +16891,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="B172" t="s">
@@ -16433,7 +16900,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
       <c r="B173" t="s">
@@ -16442,7 +16909,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
       <c r="B174" t="s">
@@ -16451,7 +16918,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
       <c r="B175" t="s">
@@ -16460,7 +16927,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="B176" t="s">
@@ -16469,7 +16936,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
       <c r="B177" t="s">
@@ -16478,7 +16945,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
       <c r="B178" t="s">
@@ -16487,7 +16954,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="B179" t="s">
@@ -16496,7 +16963,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>179</v>
       </c>
       <c r="B180" t="s">
@@ -16505,7 +16972,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="B181" t="s">
@@ -16514,7 +16981,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>181</v>
       </c>
       <c r="B182" t="s">
@@ -16523,7 +16990,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="B183" t="s">
@@ -16532,7 +16999,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>183</v>
       </c>
       <c r="B184" t="s">
@@ -16541,7 +17008,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="B185" t="s">
@@ -16550,7 +17017,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
       <c r="B186" t="s">
@@ -16559,7 +17026,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
       <c r="B187" t="s">
@@ -16568,7 +17035,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>187</v>
       </c>
       <c r="B188" t="s">
@@ -16577,7 +17044,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>188</v>
       </c>
       <c r="B189" t="s">
@@ -16586,7 +17053,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="B190" t="s">
@@ -16595,7 +17062,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="B191" t="s">
@@ -16604,7 +17071,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="B192" t="s">
@@ -16613,7 +17080,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="B193" t="s">
@@ -16622,7 +17089,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>193</v>
       </c>
       <c r="B194" t="s">
@@ -16631,7 +17098,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>194</v>
       </c>
       <c r="B195" t="s">
@@ -16640,7 +17107,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>195</v>
       </c>
       <c r="B196" t="s">
@@ -16649,7 +17116,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>196</v>
       </c>
       <c r="B197" t="s">
@@ -16658,7 +17125,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>197</v>
       </c>
       <c r="B198" t="s">
@@ -16667,7 +17134,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>198</v>
       </c>
       <c r="B199" t="s">
@@ -16676,7 +17143,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>199</v>
       </c>
       <c r="B200" t="s">
@@ -16685,7 +17152,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="B201" t="s">
@@ -16694,7 +17161,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>201</v>
       </c>
       <c r="B202" t="s">
@@ -16703,7 +17170,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>202</v>
       </c>
       <c r="B203" t="s">
@@ -16712,7 +17179,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>203</v>
       </c>
       <c r="B204" t="s">
@@ -16721,7 +17188,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="B205" t="s">
@@ -16730,7 +17197,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>205</v>
       </c>
       <c r="B206" t="s">
@@ -16739,7 +17206,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>206</v>
       </c>
       <c r="B207" t="s">
@@ -16748,6 +17215,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16756,7 +17224,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added more to developer sheet and created tables
</commit_message>
<xml_diff>
--- a/Video Games.xlsx
+++ b/Video Games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Video-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAEE603-74AD-44E3-8FA9-D12026A1C440}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDFC6D0-AA92-41FC-B2A1-1778023104BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
+    <workbookView xWindow="11700" yWindow="2370" windowWidth="7500" windowHeight="6000" firstSheet="2" activeTab="3" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
   </bookViews>
   <sheets>
     <sheet name="video_games" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="752">
   <si>
     <t>Name</t>
   </si>
@@ -2209,6 +2209,90 @@
   </si>
   <si>
     <t>Ōta, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Milan, Italy</t>
+  </si>
+  <si>
+    <t>Toronto, Canada</t>
+  </si>
+  <si>
+    <t>Montreuil, France</t>
+  </si>
+  <si>
+    <t>Frankfurt, Germany</t>
+  </si>
+  <si>
+    <t>Brighton, England</t>
+  </si>
+  <si>
+    <t>Dallas, Texas, U.S.</t>
+  </si>
+  <si>
+    <t>Madison, Wisconsin, U.S.</t>
+  </si>
+  <si>
+    <t>Kirkland, Washington, United States</t>
+  </si>
+  <si>
+    <t>Bellevue, Washington, US</t>
+  </si>
+  <si>
+    <t>Carlsbad, California, US</t>
+  </si>
+  <si>
+    <t>Chicago, US</t>
+  </si>
+  <si>
+    <t>Liverpool, England</t>
+  </si>
+  <si>
+    <t>Yodogawa-ku, Osaka, Japan</t>
+  </si>
+  <si>
+    <t>Greater New York Area, East Coast, Northeastern US</t>
+  </si>
+  <si>
+    <t>Shanghai, China</t>
+  </si>
+  <si>
+    <t>Lemont, Illinois</t>
+  </si>
+  <si>
+    <t>Manhattan Beach, California, US</t>
+  </si>
+  <si>
+    <t>Los Angeles, California</t>
+  </si>
+  <si>
+    <t>San Mateo, California</t>
+  </si>
+  <si>
+    <t>23 September 1889</t>
+  </si>
+  <si>
+    <t>11-1 Kamitoba Hokodatecho, Minami-ku, Kyoto, Japan</t>
+  </si>
+  <si>
+    <t>Shinagawa City, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Wellington, New Zealand</t>
+  </si>
+  <si>
+    <t>Kyoto, Japan</t>
+  </si>
+  <si>
+    <t>Shalford, United Kingdom</t>
+  </si>
+  <si>
+    <t>New Taipei, Taiwan</t>
+  </si>
+  <si>
+    <t>Suginami, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Ageo, Saitama, Japan</t>
   </si>
 </sst>
 </file>
@@ -2250,7 +2334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2258,6 +2342,9 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2574,8 +2661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58CEA45-1A97-47FC-8ACE-673891E6166E}">
   <dimension ref="A1:I410"/>
   <sheetViews>
-    <sheetView topLeftCell="B78" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14571,7 +14658,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15008,8 +15095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85547471-D81A-4F7D-B243-B5E5EB852E1E}">
   <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15901,6 +15988,12 @@
       <c r="B61" t="s">
         <v>205</v>
       </c>
+      <c r="C61" t="s">
+        <v>724</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1998</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
@@ -15910,6 +16003,12 @@
       <c r="B62" t="s">
         <v>208</v>
       </c>
+      <c r="C62" t="s">
+        <v>688</v>
+      </c>
+      <c r="D62" s="1">
+        <v>39412</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
@@ -15919,6 +16018,12 @@
       <c r="B63" t="s">
         <v>210</v>
       </c>
+      <c r="C63" t="s">
+        <v>725</v>
+      </c>
+      <c r="D63" s="1">
+        <v>40422</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
@@ -15928,8 +16033,14 @@
       <c r="B64" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64" t="s">
+        <v>726</v>
+      </c>
+      <c r="D64" s="1">
+        <v>31499</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -15937,8 +16048,14 @@
       <c r="B65" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>727</v>
+      </c>
+      <c r="D65" s="1">
+        <v>36404</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -15946,8 +16063,14 @@
       <c r="B66" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>728</v>
+      </c>
+      <c r="D66" s="1">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -15955,8 +16078,14 @@
       <c r="B67" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>729</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" ref="A68:A99" si="2">A67+1</f>
         <v>67</v>
@@ -15964,8 +16093,14 @@
       <c r="B68" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>730</v>
+      </c>
+      <c r="D68" s="1">
+        <v>35704</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -15973,8 +16108,14 @@
       <c r="B69" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>712</v>
+      </c>
+      <c r="D69" s="1">
+        <v>36708</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="2"/>
         <v>69</v>
@@ -15982,8 +16123,14 @@
       <c r="B70" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>731</v>
+      </c>
+      <c r="D70" s="1">
+        <v>34632</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -15991,8 +16138,14 @@
       <c r="B71" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71" t="s">
+        <v>732</v>
+      </c>
+      <c r="D71" s="1">
+        <v>35301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" si="2"/>
         <v>71</v>
@@ -16000,8 +16153,14 @@
       <c r="B72" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72" t="s">
+        <v>686</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -16009,8 +16168,14 @@
       <c r="B73" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73" t="s">
+        <v>733</v>
+      </c>
+      <c r="D73" s="1">
+        <v>30682</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -16018,8 +16183,14 @@
       <c r="B74" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74" t="s">
+        <v>711</v>
+      </c>
+      <c r="D74" s="1">
+        <v>30590</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -16027,8 +16198,14 @@
       <c r="B75" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>714</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -16036,8 +16213,14 @@
       <c r="B76" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>715</v>
+      </c>
+      <c r="D76" s="1">
+        <v>25283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -16045,8 +16228,14 @@
       <c r="B77" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>734</v>
+      </c>
+      <c r="D77" s="1">
+        <v>40288</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -16054,8 +16243,14 @@
       <c r="B78" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
+        <v>714</v>
+      </c>
+      <c r="D78" s="1">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="2"/>
         <v>78</v>
@@ -16063,8 +16258,14 @@
       <c r="B79" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>735</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="2"/>
         <v>79</v>
@@ -16072,8 +16273,11 @@
       <c r="B80" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D80" s="1">
+        <v>34095</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -16081,8 +16285,14 @@
       <c r="B81" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="D81" s="1">
+        <v>33312</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="2"/>
         <v>81</v>
@@ -16090,8 +16300,14 @@
       <c r="B82" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82" t="s">
+        <v>712</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="2"/>
         <v>82</v>
@@ -16099,8 +16315,14 @@
       <c r="B83" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
+        <v>721</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -16108,8 +16330,14 @@
       <c r="B84" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>737</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="2"/>
         <v>84</v>
@@ -16117,8 +16345,14 @@
       <c r="B85" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>738</v>
+      </c>
+      <c r="D85" s="1">
+        <v>36678</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -16126,8 +16360,14 @@
       <c r="B86" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
+        <v>739</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="2"/>
         <v>86</v>
@@ -16135,8 +16375,14 @@
       <c r="B87" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
+        <v>740</v>
+      </c>
+      <c r="D87" s="1">
+        <v>36403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="2"/>
         <v>87</v>
@@ -16144,8 +16390,14 @@
       <c r="B88" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C88" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="2"/>
         <v>88</v>
@@ -16153,8 +16405,14 @@
       <c r="B89" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C89" t="s">
+        <v>742</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="2"/>
         <v>89</v>
@@ -16162,8 +16420,14 @@
       <c r="B90" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C90" t="s">
+        <v>744</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -16171,8 +16435,14 @@
       <c r="B91" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C91" t="s">
+        <v>718</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="2"/>
         <v>91</v>
@@ -16180,8 +16450,14 @@
       <c r="B92" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C92" t="s">
+        <v>711</v>
+      </c>
+      <c r="D92" s="1">
+        <v>38777</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="2"/>
         <v>92</v>
@@ -16189,8 +16465,14 @@
       <c r="B93" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C93" t="s">
+        <v>745</v>
+      </c>
+      <c r="D93" s="1">
+        <v>35156</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="2"/>
         <v>93</v>
@@ -16198,8 +16480,14 @@
       <c r="B94" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C94" t="s">
+        <v>746</v>
+      </c>
+      <c r="D94" s="1">
+        <v>35551</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="2"/>
         <v>94</v>
@@ -16207,8 +16495,14 @@
       <c r="B95" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C95" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="D95" s="1">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -16216,8 +16510,14 @@
       <c r="B96" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C96" t="s">
+        <v>748</v>
+      </c>
+      <c r="D96" s="1">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -16225,8 +16525,14 @@
       <c r="B97" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C97" t="s">
+        <v>707</v>
+      </c>
+      <c r="D97" s="1">
+        <v>36059</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -16234,8 +16540,14 @@
       <c r="B98" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>749</v>
+      </c>
+      <c r="D98" s="1">
+        <v>32813</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="2"/>
         <v>98</v>
@@ -16243,8 +16555,14 @@
       <c r="B99" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>750</v>
+      </c>
+      <c r="D99" s="1">
+        <v>27870</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" ref="A100:A131" si="3">A99+1</f>
         <v>99</v>
@@ -16252,8 +16570,14 @@
       <c r="B100" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>751</v>
+      </c>
+      <c r="D100" s="1">
+        <v>29403</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -16262,7 +16586,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -16271,7 +16595,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -16280,7 +16604,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -16289,7 +16613,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -16298,7 +16622,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -16307,7 +16631,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -16316,7 +16640,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -16325,7 +16649,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -16334,7 +16658,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -16343,7 +16667,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -16352,7 +16676,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -17223,8 +17547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8516E1C-B839-4540-B57D-AB7AB84E8375}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added more to developer sheet
</commit_message>
<xml_diff>
--- a/Video Games.xlsx
+++ b/Video Games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajord\Video-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDFC6D0-AA92-41FC-B2A1-1778023104BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861E4418-4285-4429-B64B-2800B43DC01E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="2370" windowWidth="7500" windowHeight="6000" firstSheet="2" activeTab="3" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F96DE9BD-9C08-4A04-9D0C-C0CEC9B86860}"/>
   </bookViews>
   <sheets>
     <sheet name="video_games" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="806">
   <si>
     <t>Name</t>
   </si>
@@ -1704,9 +1704,6 @@
     <t>Confidential Mission</t>
   </si>
   <si>
-    <t>Hitmaker</t>
-  </si>
-  <si>
     <t>Dynamite Cop</t>
   </si>
   <si>
@@ -1986,9 +1983,6 @@
     <t>Star Wars Battlefront II</t>
   </si>
   <si>
-    <t>EA DICE</t>
-  </si>
-  <si>
     <t>Stealth Inc 2: A Game of Clones</t>
   </si>
   <si>
@@ -2293,6 +2287,174 @@
   </si>
   <si>
     <t>Ageo, Saitama, Japan</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Akihabara, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Redwood City, California, United States</t>
+  </si>
+  <si>
+    <t>Musashino, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>California, US</t>
+  </si>
+  <si>
+    <t>Defunct</t>
+  </si>
+  <si>
+    <t>Glen Cove, New York, U.S.</t>
+  </si>
+  <si>
+    <t>San Rafael, California, U.S.</t>
+  </si>
+  <si>
+    <t>Toyko, Japan</t>
+  </si>
+  <si>
+    <t>Nakameguro GT Tower, 2-1-1 Kamimeguro, Meguro, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Chiyoda, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Nakano, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Kōnan, Aichi, Japan</t>
+  </si>
+  <si>
+    <t>Sasebo, Nagasaki, Japan</t>
+  </si>
+  <si>
+    <t>Shinjuku, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Aalborg, Denmark</t>
+  </si>
+  <si>
+    <t>El Segundo, California</t>
+  </si>
+  <si>
+    <t>Mita, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Liverpool, England, UK</t>
+  </si>
+  <si>
+    <t>Seoul, South Korea</t>
+  </si>
+  <si>
+    <t>Shibuya, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Chicago, Illinois, U.S.</t>
+  </si>
+  <si>
+    <t>Sapporo, Hokkaido</t>
+  </si>
+  <si>
+    <t>Shibuya, Tokyo</t>
+  </si>
+  <si>
+    <t>San Diego, California, U.S.</t>
+  </si>
+  <si>
+    <t>Setagaya, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Nakano, Tokyo</t>
+  </si>
+  <si>
+    <t>Shinagawa-ku, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Shinjuku-ku, Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Derby, England, United Kingdom</t>
+  </si>
+  <si>
+    <t>Guildford, England</t>
+  </si>
+  <si>
+    <t>Yokohama, Kanagawa, Japan</t>
+  </si>
+  <si>
+    <t>Burbank, California, USA</t>
+  </si>
+  <si>
+    <t>Salt Lake City, US</t>
+  </si>
+  <si>
+    <t>Seongnam-si, South Korea</t>
+  </si>
+  <si>
+    <t>March 2, 2013</t>
+  </si>
+  <si>
+    <t>Santa Monica, California, U.S.</t>
+  </si>
+  <si>
+    <t>Sherman Oaks, California, U.S.</t>
+  </si>
+  <si>
+    <t>Seattle, Washington, US</t>
+  </si>
+  <si>
+    <t>Atlanta, Georgia, US</t>
+  </si>
+  <si>
+    <t>Vancouver, British Columbia</t>
+  </si>
+  <si>
+    <t>Gunwharf Quays, Portsmouth, England</t>
+  </si>
+  <si>
+    <t>London, England</t>
+  </si>
+  <si>
+    <t>Bellevue, Washington, United States</t>
+  </si>
+  <si>
+    <t>Partnership House, Newcastle upon Tyne, England</t>
+  </si>
+  <si>
+    <t>Southam, England</t>
+  </si>
+  <si>
+    <t>San Diego, California, U.S</t>
+  </si>
+  <si>
+    <t>Seattle, Washington, U.S.</t>
+  </si>
+  <si>
+    <t>Helsinki, Finland</t>
+  </si>
+  <si>
+    <t>San Diego, US</t>
+  </si>
+  <si>
+    <t>Boston, Massachusetts, U.S.</t>
+  </si>
+  <si>
+    <t>Montréal, Quebec, Canada</t>
+  </si>
+  <si>
+    <t>London, Ontario, Canada</t>
+  </si>
+  <si>
+    <t>Fort Lauderdale, Florida, U.S.</t>
+  </si>
+  <si>
+    <t>Gothenburg, Sweden</t>
+  </si>
+  <si>
+    <t>Oxford, England</t>
   </si>
 </sst>
 </file>
@@ -2334,7 +2496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2345,6 +2507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2661,8 +2824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58CEA45-1A97-47FC-8ACE-673891E6166E}">
   <dimension ref="A1:I410"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E277" sqref="E277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2859,7 +3022,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C7" s="1">
         <v>43763</v>
@@ -2889,7 +3052,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C8" s="1">
         <v>41947</v>
@@ -2949,7 +3112,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C10" s="1">
         <v>42404</v>
@@ -2979,7 +3142,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C11" s="1">
         <v>42314</v>
@@ -3009,7 +3172,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C12" s="1">
         <v>43385</v>
@@ -3099,7 +3262,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C15" s="1">
         <v>43042</v>
@@ -3159,7 +3322,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C17" s="1">
         <v>42549</v>
@@ -3369,7 +3532,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C24" s="1">
         <v>40624</v>
@@ -3489,7 +3652,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C28" s="1">
         <v>41338</v>
@@ -3609,7 +3772,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C32" s="1">
         <v>40855</v>
@@ -3639,7 +3802,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C33" s="1">
         <v>40127</v>
@@ -3669,7 +3832,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C34" s="1">
         <v>41583</v>
@@ -3759,7 +3922,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C37" s="1">
         <v>38524</v>
@@ -3849,7 +4012,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C40" s="1">
         <v>37210</v>
@@ -3909,7 +4072,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C42" s="1">
         <v>111425</v>
@@ -3969,7 +4132,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C44" s="1">
         <v>37943</v>
@@ -3999,7 +4162,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C45" s="1">
         <v>37957</v>
@@ -4119,7 +4282,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C49" s="1">
         <v>38460</v>
@@ -5505,7 +5668,7 @@
         <v>38271</v>
       </c>
       <c r="D95" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E95" t="s">
         <v>192</v>
@@ -5535,7 +5698,7 @@
         <v>38622</v>
       </c>
       <c r="D96" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E96" t="s">
         <v>192</v>
@@ -5925,7 +6088,7 @@
         <v>40486</v>
       </c>
       <c r="D109" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E109" t="s">
         <v>212</v>
@@ -5985,7 +6148,7 @@
         <v>40952</v>
       </c>
       <c r="D111" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E111" t="s">
         <v>216</v>
@@ -7425,7 +7588,7 @@
         <v>37337</v>
       </c>
       <c r="D159" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E159" t="s">
         <v>144</v>
@@ -7785,7 +7948,7 @@
         <v>39589</v>
       </c>
       <c r="D171" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E171" t="s">
         <v>305</v>
@@ -9741,7 +9904,7 @@
         <v>35999</v>
       </c>
       <c r="D243" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E243" t="s">
         <v>144</v>
@@ -11913,7 +12076,7 @@
         <v>36510</v>
       </c>
       <c r="D319" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E319" t="s">
         <v>482</v>
@@ -11943,7 +12106,7 @@
         <v>36643</v>
       </c>
       <c r="D320" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E320" t="s">
         <v>252</v>
@@ -12270,7 +12433,7 @@
         <v>36573</v>
       </c>
       <c r="D331" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E331" t="s">
         <v>252</v>
@@ -12570,7 +12733,7 @@
         <v>36066</v>
       </c>
       <c r="D341" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E341" t="s">
         <v>543</v>
@@ -12831,7 +12994,7 @@
         <v>43</v>
       </c>
       <c r="E350" t="s">
-        <v>555</v>
+        <v>394</v>
       </c>
       <c r="F350" t="s">
         <v>22</v>
@@ -12852,7 +13015,7 @@
         <v>350</v>
       </c>
       <c r="B351" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C351" s="1">
         <v>36307</v>
@@ -12882,7 +13045,7 @@
         <v>351</v>
       </c>
       <c r="B352" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C352" s="1">
         <v>36370</v>
@@ -12891,7 +13054,7 @@
         <v>104</v>
       </c>
       <c r="E352" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F352" t="s">
         <v>22</v>
@@ -12912,7 +13075,7 @@
         <v>352</v>
       </c>
       <c r="B353" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C353" s="1">
         <v>36877</v>
@@ -12942,7 +13105,7 @@
         <v>353</v>
       </c>
       <c r="B354" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C354" s="1">
         <v>36251</v>
@@ -12951,7 +13114,7 @@
         <v>45</v>
       </c>
       <c r="E354" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F354" t="s">
         <v>22</v>
@@ -12972,7 +13135,7 @@
         <v>354</v>
       </c>
       <c r="B355" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C355" s="1">
         <v>40120</v>
@@ -12981,7 +13144,7 @@
         <v>42</v>
       </c>
       <c r="E355" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F355" t="s">
         <v>437</v>
@@ -13002,7 +13165,7 @@
         <v>355</v>
       </c>
       <c r="B356" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C356" s="1">
         <v>39317</v>
@@ -13032,7 +13195,7 @@
         <v>356</v>
       </c>
       <c r="B357" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C357" s="1">
         <v>38608</v>
@@ -13062,7 +13225,7 @@
         <v>357</v>
       </c>
       <c r="B358" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C358" s="1">
         <v>38461</v>
@@ -13071,7 +13234,7 @@
         <v>46</v>
       </c>
       <c r="E358" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F358" t="s">
         <v>437</v>
@@ -13092,7 +13255,7 @@
         <v>358</v>
       </c>
       <c r="B359" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C359" s="1">
         <v>38435</v>
@@ -13101,7 +13264,7 @@
         <v>46</v>
       </c>
       <c r="E359" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F359" t="s">
         <v>437</v>
@@ -13122,7 +13285,7 @@
         <v>359</v>
       </c>
       <c r="B360" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C360" s="1">
         <v>39251</v>
@@ -13152,7 +13315,7 @@
         <v>360</v>
       </c>
       <c r="B361" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C361" s="1">
         <v>42710</v>
@@ -13161,7 +13324,7 @@
         <v>45</v>
       </c>
       <c r="E361" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F361" t="s">
         <v>7</v>
@@ -13182,7 +13345,7 @@
         <v>361</v>
       </c>
       <c r="B362" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C362" s="1">
         <v>42584</v>
@@ -13191,7 +13354,7 @@
         <v>104</v>
       </c>
       <c r="E362" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F362" t="s">
         <v>7</v>
@@ -13212,7 +13375,7 @@
         <v>362</v>
       </c>
       <c r="B363" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C363" s="1">
         <v>43500</v>
@@ -13221,7 +13384,7 @@
         <v>43</v>
       </c>
       <c r="E363" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F363" t="s">
         <v>7</v>
@@ -13242,7 +13405,7 @@
         <v>363</v>
       </c>
       <c r="B364" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C364" s="1">
         <v>41593</v>
@@ -13251,7 +13414,7 @@
         <v>43</v>
       </c>
       <c r="E364" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F364" t="s">
         <v>7</v>
@@ -13272,7 +13435,7 @@
         <v>364</v>
       </c>
       <c r="B365" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C365" s="1">
         <v>42087</v>
@@ -13302,7 +13465,7 @@
         <v>365</v>
       </c>
       <c r="B366" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C366" s="1">
         <v>43025</v>
@@ -13311,7 +13474,7 @@
         <v>47</v>
       </c>
       <c r="E366" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F366" t="s">
         <v>7</v>
@@ -13332,7 +13495,7 @@
         <v>366</v>
       </c>
       <c r="B367" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C367" s="1">
         <v>42678</v>
@@ -13362,7 +13525,7 @@
         <v>367</v>
       </c>
       <c r="B368" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C368" s="1">
         <v>42313</v>
@@ -13371,7 +13534,7 @@
         <v>44</v>
       </c>
       <c r="E368" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F368" t="s">
         <v>7</v>
@@ -13392,7 +13555,7 @@
         <v>368</v>
       </c>
       <c r="B369" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C369" s="1">
         <v>43431</v>
@@ -13401,7 +13564,7 @@
         <v>44</v>
       </c>
       <c r="E369" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F369" t="s">
         <v>7</v>
@@ -13422,7 +13585,7 @@
         <v>369</v>
       </c>
       <c r="B370" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C370" s="1">
         <v>42703</v>
@@ -13431,7 +13594,7 @@
         <v>44</v>
       </c>
       <c r="E370" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F370" t="s">
         <v>7</v>
@@ -13452,7 +13615,7 @@
         <v>370</v>
       </c>
       <c r="B371" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C371" s="1">
         <v>43734</v>
@@ -13461,7 +13624,7 @@
         <v>44</v>
       </c>
       <c r="E371" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F371" t="s">
         <v>7</v>
@@ -13482,7 +13645,7 @@
         <v>371</v>
       </c>
       <c r="B372" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C372" s="1">
         <v>41593</v>
@@ -13491,7 +13654,7 @@
         <v>42</v>
       </c>
       <c r="E372" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F372" t="s">
         <v>7</v>
@@ -13512,7 +13675,7 @@
         <v>372</v>
       </c>
       <c r="B373" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C373" s="1">
         <v>42535</v>
@@ -13521,7 +13684,7 @@
         <v>42</v>
       </c>
       <c r="E373" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F373" t="s">
         <v>7</v>
@@ -13542,7 +13705,7 @@
         <v>373</v>
       </c>
       <c r="B374" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C374" s="2">
         <v>41702</v>
@@ -13551,7 +13714,7 @@
         <v>43</v>
       </c>
       <c r="E374" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F374" t="s">
         <v>7</v>
@@ -13572,7 +13735,7 @@
         <v>374</v>
       </c>
       <c r="B375" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C375" s="1">
         <v>44047</v>
@@ -13581,7 +13744,7 @@
         <v>42</v>
       </c>
       <c r="E375" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F375" t="s">
         <v>7</v>
@@ -13602,7 +13765,7 @@
         <v>375</v>
       </c>
       <c r="B376" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C376" s="1">
         <v>42780</v>
@@ -13632,7 +13795,7 @@
         <v>376</v>
       </c>
       <c r="B377" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C377" s="1">
         <v>42941</v>
@@ -13662,7 +13825,7 @@
         <v>377</v>
       </c>
       <c r="B378" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C378" s="1">
         <v>42227</v>
@@ -13671,7 +13834,7 @@
         <v>42</v>
       </c>
       <c r="E378" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F378" t="s">
         <v>7</v>
@@ -13692,7 +13855,7 @@
         <v>378</v>
       </c>
       <c r="B379" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C379" s="1">
         <v>44029</v>
@@ -13701,7 +13864,7 @@
         <v>42</v>
       </c>
       <c r="E379" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F379" t="s">
         <v>7</v>
@@ -13722,7 +13885,7 @@
         <v>379</v>
       </c>
       <c r="B380" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C380" s="1">
         <v>42248</v>
@@ -13731,7 +13894,7 @@
         <v>42</v>
       </c>
       <c r="E380" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F380" t="s">
         <v>7</v>
@@ -13752,7 +13915,7 @@
         <v>380</v>
       </c>
       <c r="B381" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C381" s="1">
         <v>43242</v>
@@ -13761,7 +13924,7 @@
         <v>43</v>
       </c>
       <c r="E381" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F381" t="s">
         <v>7</v>
@@ -13782,7 +13945,7 @@
         <v>381</v>
       </c>
       <c r="B382" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C382" s="1">
         <v>42066</v>
@@ -13791,7 +13954,7 @@
         <v>43</v>
       </c>
       <c r="E382" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F382" t="s">
         <v>7</v>
@@ -13812,7 +13975,7 @@
         <v>382</v>
       </c>
       <c r="B383" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C383" s="1">
         <v>42692</v>
@@ -13842,7 +14005,7 @@
         <v>383</v>
       </c>
       <c r="B384" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C384" s="1">
         <v>41954</v>
@@ -13872,7 +14035,7 @@
         <v>384</v>
       </c>
       <c r="B385" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C385" s="1">
         <v>41912</v>
@@ -13902,7 +14065,7 @@
         <v>385</v>
       </c>
       <c r="B386" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C386" s="1">
         <v>43259</v>
@@ -13911,7 +14074,7 @@
         <v>46</v>
       </c>
       <c r="E386" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F386" t="s">
         <v>7</v>
@@ -13932,7 +14095,7 @@
         <v>386</v>
       </c>
       <c r="B387" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C387" s="1">
         <v>42178</v>
@@ -13941,7 +14104,7 @@
         <v>43</v>
       </c>
       <c r="E387" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F387" t="s">
         <v>7</v>
@@ -13962,7 +14125,7 @@
         <v>387</v>
       </c>
       <c r="B388" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C388" s="1">
         <v>41695</v>
@@ -13971,7 +14134,7 @@
         <v>43</v>
       </c>
       <c r="E388" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F388" t="s">
         <v>7</v>
@@ -13992,7 +14155,7 @@
         <v>388</v>
       </c>
       <c r="B389" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C389" s="1">
         <v>41593</v>
@@ -14001,7 +14164,7 @@
         <v>43</v>
       </c>
       <c r="E389" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F389" t="s">
         <v>7</v>
@@ -14022,7 +14185,7 @@
         <v>389</v>
       </c>
       <c r="B390" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C390" s="1">
         <v>42192</v>
@@ -14031,7 +14194,7 @@
         <v>45</v>
       </c>
       <c r="E390" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F390" t="s">
         <v>7</v>
@@ -14052,7 +14215,7 @@
         <v>390</v>
       </c>
       <c r="B391" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C391" s="1">
         <v>43137</v>
@@ -14061,7 +14224,7 @@
         <v>42</v>
       </c>
       <c r="E391" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F391" t="s">
         <v>7</v>
@@ -14082,7 +14245,7 @@
         <v>391</v>
       </c>
       <c r="B392" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C392" s="1">
         <v>42521</v>
@@ -14091,7 +14254,7 @@
         <v>42</v>
       </c>
       <c r="E392" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F392" t="s">
         <v>7</v>
@@ -14112,7 +14275,7 @@
         <v>392</v>
       </c>
       <c r="B393" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C393" s="1">
         <v>44008</v>
@@ -14121,7 +14284,7 @@
         <v>42</v>
       </c>
       <c r="E393" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F393" t="s">
         <v>7</v>
@@ -14142,7 +14305,7 @@
         <v>393</v>
       </c>
       <c r="B394" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C394" s="1">
         <v>43056</v>
@@ -14151,7 +14314,7 @@
         <v>43</v>
       </c>
       <c r="E394" t="s">
-        <v>649</v>
+        <v>98</v>
       </c>
       <c r="F394" t="s">
         <v>7</v>
@@ -14172,7 +14335,7 @@
         <v>394</v>
       </c>
       <c r="B395" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C395" s="1">
         <v>42101</v>
@@ -14181,7 +14344,7 @@
         <v>172</v>
       </c>
       <c r="E395" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F395" t="s">
         <v>7</v>
@@ -14202,7 +14365,7 @@
         <v>395</v>
       </c>
       <c r="B396" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C396" s="1">
         <v>42472</v>
@@ -14211,7 +14374,7 @@
         <v>44</v>
       </c>
       <c r="E396" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="F396" t="s">
         <v>7</v>
@@ -14232,7 +14395,7 @@
         <v>396</v>
       </c>
       <c r="B397" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C397" s="1">
         <v>41688</v>
@@ -14241,7 +14404,7 @@
         <v>42</v>
       </c>
       <c r="E397" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="F397" t="s">
         <v>7</v>
@@ -14262,7 +14425,7 @@
         <v>397</v>
       </c>
       <c r="B398" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C398" s="1">
         <v>41849</v>
@@ -14292,7 +14455,7 @@
         <v>398</v>
       </c>
       <c r="B399" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C399" s="1">
         <v>42500</v>
@@ -14322,7 +14485,7 @@
         <v>399</v>
       </c>
       <c r="B400" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C400" s="1">
         <v>42284</v>
@@ -14352,7 +14515,7 @@
         <v>400</v>
       </c>
       <c r="B401" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C401" s="1">
         <v>41590</v>
@@ -14361,7 +14524,7 @@
         <v>44</v>
       </c>
       <c r="E401" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="F401" t="s">
         <v>7</v>
@@ -14382,7 +14545,7 @@
         <v>401</v>
       </c>
       <c r="B402" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C402" s="1">
         <v>43571</v>
@@ -14391,7 +14554,7 @@
         <v>43</v>
       </c>
       <c r="E402" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="F402" t="s">
         <v>7</v>
@@ -14412,7 +14575,7 @@
         <v>402</v>
       </c>
       <c r="B403" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C403" s="1">
         <v>43777</v>
@@ -14421,7 +14584,7 @@
         <v>46</v>
       </c>
       <c r="E403" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F403" t="s">
         <v>7</v>
@@ -14442,7 +14605,7 @@
         <v>403</v>
       </c>
       <c r="B404" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C404" s="1">
         <v>43350</v>
@@ -14472,7 +14635,7 @@
         <v>404</v>
       </c>
       <c r="B405" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C405" s="1">
         <v>43210</v>
@@ -14502,7 +14665,7 @@
         <v>405</v>
       </c>
       <c r="B406" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C406" s="1">
         <v>43018</v>
@@ -14532,7 +14695,7 @@
         <v>406</v>
       </c>
       <c r="B407" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C407" s="1">
         <v>42248</v>
@@ -14541,7 +14704,7 @@
         <v>42</v>
       </c>
       <c r="E407" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F407" t="s">
         <v>7</v>
@@ -14562,7 +14725,7 @@
         <v>407</v>
       </c>
       <c r="B408" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C408" s="1">
         <v>41786</v>
@@ -14592,7 +14755,7 @@
         <v>408</v>
       </c>
       <c r="B409" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C409" s="1">
         <v>41821</v>
@@ -14601,7 +14764,7 @@
         <v>172</v>
       </c>
       <c r="E409" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="F409" t="s">
         <v>7</v>
@@ -14622,7 +14785,7 @@
         <v>409</v>
       </c>
       <c r="B410" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C410" s="1">
         <v>42437</v>
@@ -14787,10 +14950,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -14798,10 +14961,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -14809,10 +14972,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C13" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -15093,10 +15256,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85547471-D81A-4F7D-B243-B5E5EB852E1E}">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15107,9 +15270,9 @@
     <col min="4" max="4" width="13.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -15120,8 +15283,11 @@
       <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -15129,13 +15295,13 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D2" s="1">
         <v>38400</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -15143,13 +15309,13 @@
         <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D3" s="1">
         <v>36526</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A35" si="0">A3+1</f>
         <v>3</v>
@@ -15158,13 +15324,13 @@
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D4" s="1">
         <v>33359</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15173,13 +15339,13 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D5" s="4">
         <v>1997</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -15188,13 +15354,13 @@
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D6" s="1">
         <v>30952</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -15203,13 +15369,13 @@
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D7" s="1">
         <v>37377</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -15218,13 +15384,13 @@
         <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D8" s="1">
         <v>40015</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -15233,13 +15399,13 @@
         <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D9" s="1">
         <v>33725</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -15248,13 +15414,13 @@
         <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D10" s="1">
         <v>35111</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -15263,13 +15429,13 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D11" s="4">
         <v>1996</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -15278,13 +15444,13 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D12" s="1">
         <v>35545</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -15293,13 +15459,13 @@
         <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D13" s="1">
         <v>34393</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -15308,13 +15474,13 @@
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D14" s="1">
         <v>33270</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -15323,13 +15489,13 @@
         <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D15" s="4">
         <v>2005</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -15338,7 +15504,7 @@
         <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D16" s="4">
         <v>1989</v>
@@ -15353,7 +15519,7 @@
         <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D17" s="1">
         <v>35382</v>
@@ -15368,7 +15534,7 @@
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D18" s="1">
         <v>1991</v>
@@ -15383,7 +15549,7 @@
         <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D19" s="1">
         <v>36207</v>
@@ -15398,7 +15564,7 @@
         <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D20" s="1">
         <v>1994</v>
@@ -15413,7 +15579,7 @@
         <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D21" s="1">
         <v>1998</v>
@@ -15428,7 +15594,7 @@
         <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D22" s="1">
         <v>2007</v>
@@ -15443,7 +15609,7 @@
         <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D23" s="1">
         <v>29005</v>
@@ -15458,7 +15624,7 @@
         <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D24" s="1">
         <v>1999</v>
@@ -15473,7 +15639,7 @@
         <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D25" s="1">
         <v>1985</v>
@@ -15488,7 +15654,7 @@
         <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D26" s="1">
         <v>1999</v>
@@ -15503,7 +15669,7 @@
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D27" s="1">
         <v>1994</v>
@@ -15518,7 +15684,7 @@
         <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D28" s="1">
         <v>34578</v>
@@ -15533,7 +15699,7 @@
         <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D29" s="1">
         <v>1997</v>
@@ -15548,7 +15714,7 @@
         <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D30" s="1">
         <v>1997</v>
@@ -15563,7 +15729,7 @@
         <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D31" s="1">
         <v>35384</v>
@@ -15578,7 +15744,7 @@
         <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D32" s="1">
         <v>34731</v>
@@ -15602,7 +15768,7 @@
         <v>121</v>
       </c>
       <c r="C34" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D34" s="1">
         <v>39904</v>
@@ -15617,7 +15783,7 @@
         <v>122</v>
       </c>
       <c r="C35" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D35" s="1">
         <v>1991</v>
@@ -15632,7 +15798,7 @@
         <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D36" s="1">
         <v>28693</v>
@@ -15647,7 +15813,7 @@
         <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D37" s="1">
         <v>31717</v>
@@ -15662,7 +15828,7 @@
         <v>134</v>
       </c>
       <c r="C38" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D38" s="1">
         <v>1994</v>
@@ -15677,7 +15843,7 @@
         <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D39" s="1">
         <v>2000</v>
@@ -15692,7 +15858,7 @@
         <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D40" s="1">
         <v>1997</v>
@@ -15707,7 +15873,7 @@
         <v>143</v>
       </c>
       <c r="C41" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D41" s="1">
         <v>36586</v>
@@ -15722,7 +15888,7 @@
         <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D42" s="1">
         <v>25283</v>
@@ -15737,7 +15903,7 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D43" s="1">
         <v>1999</v>
@@ -15752,7 +15918,7 @@
         <v>149</v>
       </c>
       <c r="C44" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D44" s="1">
         <v>34043</v>
@@ -15767,7 +15933,7 @@
         <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D45" s="1">
         <v>32275</v>
@@ -15782,7 +15948,7 @@
         <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D46" s="1">
         <v>35004</v>
@@ -15806,7 +15972,7 @@
         <v>158</v>
       </c>
       <c r="C48" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D48" s="1">
         <v>29005</v>
@@ -15821,7 +15987,7 @@
         <v>165</v>
       </c>
       <c r="C49" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D49" s="1">
         <v>1996</v>
@@ -15845,7 +16011,7 @@
         <v>177</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D51" s="1">
         <v>36637</v>
@@ -15860,7 +16026,7 @@
         <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D52" s="1">
         <v>2003</v>
@@ -15875,7 +16041,7 @@
         <v>181</v>
       </c>
       <c r="C53" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D53" s="1">
         <v>2003</v>
@@ -15890,7 +16056,7 @@
         <v>184</v>
       </c>
       <c r="C54" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D54" s="1">
         <v>37575</v>
@@ -15905,7 +16071,7 @@
         <v>187</v>
       </c>
       <c r="C55" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D55" s="1">
         <v>35467</v>
@@ -15920,7 +16086,7 @@
         <v>189</v>
       </c>
       <c r="C56" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D56" s="1">
         <v>22070</v>
@@ -15935,7 +16101,7 @@
         <v>192</v>
       </c>
       <c r="C57" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D57" s="1">
         <v>2003</v>
@@ -15950,7 +16116,7 @@
         <v>195</v>
       </c>
       <c r="C58" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D58" s="1">
         <v>34060</v>
@@ -15965,7 +16131,7 @@
         <v>199</v>
       </c>
       <c r="C59" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D59" s="1">
         <v>20241</v>
@@ -15989,7 +16155,7 @@
         <v>205</v>
       </c>
       <c r="C61" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D61" s="1">
         <v>1998</v>
@@ -16004,7 +16170,7 @@
         <v>208</v>
       </c>
       <c r="C62" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D62" s="1">
         <v>39412</v>
@@ -16019,7 +16185,7 @@
         <v>210</v>
       </c>
       <c r="C63" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D63" s="1">
         <v>40422</v>
@@ -16034,7 +16200,7 @@
         <v>212</v>
       </c>
       <c r="C64" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D64" s="1">
         <v>31499</v>
@@ -16049,7 +16215,7 @@
         <v>214</v>
       </c>
       <c r="C65" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D65" s="1">
         <v>36404</v>
@@ -16064,7 +16230,7 @@
         <v>216</v>
       </c>
       <c r="C66" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D66" s="1">
         <v>2004</v>
@@ -16079,7 +16245,7 @@
         <v>223</v>
       </c>
       <c r="C67" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D67" s="1">
         <v>1994</v>
@@ -16094,7 +16260,7 @@
         <v>226</v>
       </c>
       <c r="C68" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D68" s="1">
         <v>35704</v>
@@ -16109,7 +16275,7 @@
         <v>229</v>
       </c>
       <c r="C69" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D69" s="1">
         <v>36708</v>
@@ -16124,7 +16290,7 @@
         <v>232</v>
       </c>
       <c r="C70" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D70" s="1">
         <v>34632</v>
@@ -16139,7 +16305,7 @@
         <v>238</v>
       </c>
       <c r="C71" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D71" s="1">
         <v>35301</v>
@@ -16154,7 +16320,7 @@
         <v>242</v>
       </c>
       <c r="C72" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D72" s="1">
         <v>1998</v>
@@ -16169,7 +16335,7 @@
         <v>244</v>
       </c>
       <c r="C73" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D73" s="1">
         <v>30682</v>
@@ -16184,7 +16350,7 @@
         <v>246</v>
       </c>
       <c r="C74" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D74" s="1">
         <v>30590</v>
@@ -16199,7 +16365,7 @@
         <v>248</v>
       </c>
       <c r="C75" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D75" s="1">
         <v>2007</v>
@@ -16214,7 +16380,7 @@
         <v>252</v>
       </c>
       <c r="C76" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D76" s="1">
         <v>25283</v>
@@ -16229,7 +16395,7 @@
         <v>255</v>
       </c>
       <c r="C77" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D77" s="1">
         <v>40288</v>
@@ -16244,7 +16410,7 @@
         <v>257</v>
       </c>
       <c r="C78" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D78" s="1">
         <v>2009</v>
@@ -16259,7 +16425,7 @@
         <v>263</v>
       </c>
       <c r="C79" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D79" s="1">
         <v>1988</v>
@@ -16286,7 +16452,7 @@
         <v>272</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D81" s="1">
         <v>33312</v>
@@ -16301,7 +16467,7 @@
         <v>276</v>
       </c>
       <c r="C82" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D82" s="1">
         <v>1988</v>
@@ -16316,7 +16482,7 @@
         <v>278</v>
       </c>
       <c r="C83" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D83" s="1">
         <v>1992</v>
@@ -16331,7 +16497,7 @@
         <v>281</v>
       </c>
       <c r="C84" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D84" s="1">
         <v>1995</v>
@@ -16346,7 +16512,7 @@
         <v>283</v>
       </c>
       <c r="C85" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D85" s="1">
         <v>36678</v>
@@ -16361,7 +16527,7 @@
         <v>286</v>
       </c>
       <c r="C86" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D86" s="1">
         <v>1993</v>
@@ -16376,7 +16542,7 @@
         <v>289</v>
       </c>
       <c r="C87" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D87" s="1">
         <v>36403</v>
@@ -16391,7 +16557,7 @@
         <v>291</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D88" s="1">
         <v>1997</v>
@@ -16406,7 +16572,7 @@
         <v>294</v>
       </c>
       <c r="C89" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D89" s="1">
         <v>1994</v>
@@ -16421,10 +16587,10 @@
         <v>11</v>
       </c>
       <c r="C90" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
@@ -16436,7 +16602,7 @@
         <v>297</v>
       </c>
       <c r="C91" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D91" s="1">
         <v>1977</v>
@@ -16451,7 +16617,7 @@
         <v>299</v>
       </c>
       <c r="C92" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D92" s="1">
         <v>38777</v>
@@ -16466,7 +16632,7 @@
         <v>301</v>
       </c>
       <c r="C93" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D93" s="1">
         <v>35156</v>
@@ -16481,7 +16647,7 @@
         <v>303</v>
       </c>
       <c r="C94" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D94" s="1">
         <v>35551</v>
@@ -16496,7 +16662,7 @@
         <v>305</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D95" s="1">
         <v>2004</v>
@@ -16511,13 +16677,13 @@
         <v>310</v>
       </c>
       <c r="C96" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D96" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -16526,13 +16692,13 @@
         <v>312</v>
       </c>
       <c r="C97" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D97" s="1">
         <v>36059</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -16541,13 +16707,13 @@
         <v>315</v>
       </c>
       <c r="C98" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D98" s="1">
         <v>32813</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="2"/>
         <v>98</v>
@@ -16556,28 +16722,28 @@
         <v>318</v>
       </c>
       <c r="C99" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D99" s="1">
         <v>27870</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
-        <f t="shared" ref="A100:A131" si="3">A99+1</f>
+        <f t="shared" ref="A100:A163" si="3">A99+1</f>
         <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>326</v>
       </c>
       <c r="C100" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D100" s="1">
         <v>29403</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -16585,8 +16751,14 @@
       <c r="B101" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C101" t="s">
+        <v>750</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -16594,8 +16766,14 @@
       <c r="B102" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C102" t="s">
+        <v>710</v>
+      </c>
+      <c r="D102" s="1">
+        <v>31168</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -16603,8 +16781,14 @@
       <c r="B103" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C103" t="s">
+        <v>710</v>
+      </c>
+      <c r="D103" s="1">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -16612,8 +16796,14 @@
       <c r="B104" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>697</v>
+      </c>
+      <c r="D104" s="1">
+        <v>29005</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -16621,8 +16811,14 @@
       <c r="B105" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C105" t="s">
+        <v>751</v>
+      </c>
+      <c r="D105" s="1">
+        <v>35158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -16630,8 +16826,14 @@
       <c r="B106" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C106" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="D106" s="1">
+        <v>33793</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -16639,8 +16841,14 @@
       <c r="B107" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C107" t="s">
+        <v>753</v>
+      </c>
+      <c r="D107" s="1">
+        <v>34869</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -16648,8 +16856,17 @@
       <c r="B108" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C108" t="s">
+        <v>754</v>
+      </c>
+      <c r="D108" s="1">
+        <v>36708</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -16657,8 +16874,17 @@
       <c r="B109" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C109" t="s">
+        <v>756</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1987</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -16666,8 +16892,17 @@
       <c r="B110" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C110" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1987</v>
+      </c>
+      <c r="E110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -16675,8 +16910,17 @@
       <c r="B111" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C111" t="s">
+        <v>710</v>
+      </c>
+      <c r="D111" s="1">
+        <v>38169</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -16684,8 +16928,17 @@
       <c r="B112" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C112" t="s">
+        <v>758</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1986</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>112</v>
@@ -16693,8 +16946,14 @@
       <c r="B113" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C113" t="s">
+        <v>759</v>
+      </c>
+      <c r="D113" s="1">
+        <v>36434</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -16702,8 +16961,14 @@
       <c r="B114" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C114" t="s">
+        <v>760</v>
+      </c>
+      <c r="D114" s="1">
+        <v>35884</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -16711,8 +16976,17 @@
       <c r="B115" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C115" t="s">
+        <v>745</v>
+      </c>
+      <c r="D115" s="1">
+        <v>31017</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -16720,8 +16994,17 @@
       <c r="B116" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C116" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="D116" s="1">
+        <v>29921</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -16729,8 +17012,14 @@
       <c r="B117" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C117" t="s">
+        <v>762</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -16738,8 +17027,17 @@
       <c r="B118" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C118" t="s">
+        <v>763</v>
+      </c>
+      <c r="D118" s="1">
+        <v>29252</v>
+      </c>
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -16747,8 +17045,17 @@
       <c r="B119" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C119" t="s">
+        <v>710</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1993</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -16756,8 +17063,14 @@
       <c r="B120" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C120" t="s">
+        <v>758</v>
+      </c>
+      <c r="D120" s="1">
+        <v>33774</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>120</v>
@@ -16765,8 +17078,17 @@
       <c r="B121" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C121" t="s">
+        <v>745</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1992</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -16774,8 +17096,14 @@
       <c r="B122" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C122" t="s">
+        <v>715</v>
+      </c>
+      <c r="D122" s="1">
+        <v>22070</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -16783,758 +17111,1262 @@
       <c r="B123" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C123" t="s">
+        <v>764</v>
+      </c>
+      <c r="D123" s="1">
+        <v>34700</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+        <v>412</v>
+      </c>
+      <c r="C124" t="s">
+        <v>745</v>
+      </c>
+      <c r="D124" s="1">
+        <v>29160</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+        <v>421</v>
+      </c>
+      <c r="C125" t="s">
+        <v>765</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+      <c r="C126" t="s">
+        <v>710</v>
+      </c>
+      <c r="D126" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+        <v>426</v>
+      </c>
+      <c r="C127" t="s">
+        <v>758</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+        <v>428</v>
+      </c>
+      <c r="C128" t="s">
+        <v>764</v>
+      </c>
+      <c r="D128" s="1">
+        <v>19595</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+        <v>431</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="D129" s="1">
+        <v>34428</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+      <c r="C130" t="s">
+        <v>760</v>
+      </c>
+      <c r="D130" s="1">
+        <v>27220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+        <v>435</v>
+      </c>
+      <c r="C131" t="s">
+        <v>766</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132">
-        <f t="shared" ref="A132:A150" si="4">A131+1</f>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+        <v>441</v>
+      </c>
+      <c r="C132" t="s">
+        <v>767</v>
+      </c>
+      <c r="D132" s="1">
+        <v>35159</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>447</v>
+      </c>
+      <c r="C133" t="s">
+        <v>764</v>
+      </c>
+      <c r="D133" s="1">
+        <v>1994</v>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <f t="shared" si="3"/>
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>451</v>
+      </c>
+      <c r="C134" t="s">
+        <v>710</v>
+      </c>
+      <c r="D134" s="1">
+        <v>36637</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <f t="shared" si="3"/>
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>453</v>
+      </c>
+      <c r="C135" t="s">
+        <v>768</v>
+      </c>
+      <c r="D135" s="1">
+        <v>1992</v>
+      </c>
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>472</v>
+      </c>
+      <c r="C136" t="s">
+        <v>697</v>
+      </c>
+      <c r="D136" s="1">
+        <v>29005</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <f t="shared" si="3"/>
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>474</v>
+      </c>
+      <c r="C137" t="s">
+        <v>769</v>
+      </c>
+      <c r="D137" s="1">
+        <v>37362</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <f t="shared" si="3"/>
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>477</v>
+      </c>
+      <c r="C138" t="s">
+        <v>710</v>
+      </c>
+      <c r="D138" s="1">
+        <v>36637</v>
+      </c>
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <f t="shared" si="3"/>
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>479</v>
+      </c>
+      <c r="C139" t="s">
+        <v>743</v>
+      </c>
+      <c r="D139" s="1">
+        <v>35156</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <f t="shared" si="3"/>
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>482</v>
+      </c>
+      <c r="C140" t="s">
+        <v>770</v>
+      </c>
+      <c r="D140" s="1">
+        <v>1996</v>
+      </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>485</v>
+      </c>
+      <c r="C141" t="s">
+        <v>710</v>
+      </c>
+      <c r="D141" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <f t="shared" si="3"/>
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>487</v>
+      </c>
+      <c r="C142" t="s">
+        <v>771</v>
+      </c>
+      <c r="D142" s="1">
+        <v>1958</v>
+      </c>
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <f t="shared" si="3"/>
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>489</v>
+      </c>
+      <c r="C143" t="s">
+        <v>710</v>
+      </c>
+      <c r="D143" s="1">
+        <v>30048</v>
+      </c>
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <f t="shared" si="3"/>
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>492</v>
+      </c>
+      <c r="C144" t="s">
+        <v>710</v>
+      </c>
+      <c r="D144" s="1">
+        <v>32203</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>494</v>
+      </c>
+      <c r="C145" t="s">
+        <v>772</v>
+      </c>
+      <c r="D145" s="1">
+        <v>32264</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <f t="shared" si="3"/>
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>500</v>
+      </c>
+      <c r="C146" t="s">
+        <v>758</v>
+      </c>
+      <c r="D146" s="1">
+        <v>32546</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <f t="shared" si="3"/>
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>502</v>
+      </c>
+      <c r="C147" t="s">
+        <v>709</v>
+      </c>
+      <c r="D147" s="1">
+        <v>28648</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <f t="shared" si="3"/>
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>505</v>
+      </c>
+      <c r="C148" t="s">
+        <v>710</v>
+      </c>
+      <c r="D148" s="1">
+        <v>34096</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <f t="shared" si="3"/>
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>509</v>
+      </c>
+      <c r="C149" t="s">
+        <v>710</v>
+      </c>
+      <c r="D149" s="1">
+        <v>35400</v>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <f t="shared" si="3"/>
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>512</v>
+      </c>
+      <c r="C150" t="s">
+        <v>758</v>
+      </c>
+      <c r="D150" s="1">
+        <v>1985</v>
+      </c>
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>514</v>
+      </c>
+      <c r="C151" t="s">
+        <v>773</v>
+      </c>
+      <c r="D151" s="1">
+        <v>30590</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <f t="shared" si="3"/>
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>518</v>
+      </c>
+      <c r="C152" t="s">
+        <v>774</v>
+      </c>
+      <c r="D152" s="1">
+        <v>1997</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <f t="shared" si="3"/>
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>521</v>
+      </c>
+      <c r="C153" t="s">
+        <v>775</v>
+      </c>
+      <c r="D153" s="1">
+        <v>31509</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>523</v>
+      </c>
+      <c r="C154" t="s">
+        <v>776</v>
+      </c>
+      <c r="D154" s="1">
+        <v>33162</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>527</v>
+      </c>
+      <c r="C155" t="s">
+        <v>758</v>
+      </c>
+      <c r="D155" s="1">
+        <v>34397</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <f t="shared" si="3"/>
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>529</v>
+      </c>
+      <c r="C156" t="s">
+        <v>777</v>
+      </c>
+      <c r="D156" s="1">
+        <v>27305</v>
+      </c>
+      <c r="E156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <f t="shared" si="3"/>
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>531</v>
+      </c>
+      <c r="C157" t="s">
+        <v>778</v>
+      </c>
+      <c r="D157" s="1">
+        <v>1995</v>
+      </c>
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <f t="shared" si="3"/>
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>533</v>
+      </c>
+      <c r="C158" t="s">
+        <v>779</v>
+      </c>
+      <c r="D158" s="1">
+        <v>32417</v>
+      </c>
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <f t="shared" si="3"/>
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>536</v>
+      </c>
+      <c r="C159" t="s">
+        <v>710</v>
+      </c>
+      <c r="D159" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <f t="shared" si="3"/>
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>538</v>
+      </c>
+      <c r="C160" t="s">
+        <v>710</v>
+      </c>
+      <c r="D160" s="1">
+        <v>1991</v>
+      </c>
+      <c r="E160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>541</v>
+      </c>
+      <c r="C161" t="s">
+        <v>724</v>
+      </c>
+      <c r="D161" s="1">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <f t="shared" si="3"/>
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>543</v>
+      </c>
+      <c r="C162" t="s">
+        <v>709</v>
+      </c>
+      <c r="D162" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <f t="shared" si="3"/>
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>545</v>
+      </c>
+      <c r="C163" t="s">
+        <v>780</v>
+      </c>
+      <c r="D163" s="1">
+        <v>35065</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <f t="shared" ref="A164:A202" si="4">A163+1</f>
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>547</v>
+      </c>
+      <c r="C164" t="s">
+        <v>760</v>
+      </c>
+      <c r="D164" s="1">
+        <v>31108</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165">
         <f t="shared" si="4"/>
-        <v>132</v>
-      </c>
-      <c r="B133" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>537</v>
+      </c>
+      <c r="C165" t="s">
+        <v>710</v>
+      </c>
+      <c r="D165" s="1">
+        <v>1993</v>
+      </c>
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166">
         <f t="shared" si="4"/>
-        <v>133</v>
-      </c>
-      <c r="B134" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>557</v>
+      </c>
+      <c r="C166" t="s">
+        <v>781</v>
+      </c>
+      <c r="D166" s="1">
+        <v>35490</v>
+      </c>
+      <c r="E166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167">
         <f t="shared" si="4"/>
-        <v>134</v>
-      </c>
-      <c r="B135" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>560</v>
+      </c>
+      <c r="C167" t="s">
+        <v>770</v>
+      </c>
+      <c r="D167" s="1">
+        <v>33401</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168">
         <f t="shared" si="4"/>
-        <v>135</v>
-      </c>
-      <c r="B136" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>562</v>
+      </c>
+      <c r="C168" t="s">
+        <v>782</v>
+      </c>
+      <c r="D168" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169">
         <f t="shared" si="4"/>
-        <v>136</v>
-      </c>
-      <c r="B137" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>566</v>
+      </c>
+      <c r="C169" t="s">
+        <v>695</v>
+      </c>
+      <c r="D169" s="1">
+        <v>2004</v>
+      </c>
+      <c r="E169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170">
         <f t="shared" si="4"/>
-        <v>137</v>
-      </c>
-      <c r="B138" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>568</v>
+      </c>
+      <c r="C170" t="s">
+        <v>783</v>
+      </c>
+      <c r="D170" s="1">
+        <v>1999</v>
+      </c>
+      <c r="E170" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171">
         <f t="shared" si="4"/>
-        <v>138</v>
-      </c>
-      <c r="B139" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>591</v>
+      </c>
+      <c r="C171" t="s">
+        <v>784</v>
+      </c>
+      <c r="D171" s="1">
+        <v>34484</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172">
         <f t="shared" si="4"/>
-        <v>139</v>
-      </c>
-      <c r="B140" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>593</v>
+      </c>
+      <c r="C172" t="s">
+        <v>786</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173">
         <f t="shared" si="4"/>
-        <v>140</v>
-      </c>
-      <c r="B141" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>595</v>
+      </c>
+      <c r="C173" t="s">
+        <v>787</v>
+      </c>
+      <c r="D173" s="1">
+        <v>40280</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174">
         <f t="shared" si="4"/>
-        <v>141</v>
-      </c>
-      <c r="B142" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>597</v>
+      </c>
+      <c r="C174" t="s">
+        <v>788</v>
+      </c>
+      <c r="D174" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175">
         <f t="shared" si="4"/>
-        <v>142</v>
-      </c>
-      <c r="B143" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>600</v>
+      </c>
+      <c r="C175" t="s">
+        <v>789</v>
+      </c>
+      <c r="D175" s="1">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176">
         <f t="shared" si="4"/>
-        <v>143</v>
-      </c>
-      <c r="B144" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>603</v>
+      </c>
+      <c r="C176" t="s">
+        <v>705</v>
+      </c>
+      <c r="D176" s="1">
+        <v>2005</v>
+      </c>
+      <c r="E176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <f>A176+1</f>
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>605</v>
+      </c>
+      <c r="C177" t="s">
+        <v>705</v>
+      </c>
+      <c r="D177" s="1">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178">
         <f t="shared" si="4"/>
-        <v>144</v>
-      </c>
-      <c r="B145" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>608</v>
+      </c>
+      <c r="C178" t="s">
+        <v>790</v>
+      </c>
+      <c r="D178" s="1">
+        <v>41730</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179">
         <f t="shared" si="4"/>
-        <v>145</v>
-      </c>
-      <c r="B146" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
+        <v>610</v>
+      </c>
+      <c r="C179" t="s">
+        <v>705</v>
+      </c>
+      <c r="D179" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180">
         <f t="shared" si="4"/>
-        <v>146</v>
-      </c>
-      <c r="B147" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
+        <v>612</v>
+      </c>
+      <c r="C180" t="s">
+        <v>686</v>
+      </c>
+      <c r="D180" s="1">
+        <v>33868</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181">
         <f t="shared" si="4"/>
-        <v>147</v>
-      </c>
-      <c r="B148" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
+        <v>614</v>
+      </c>
+      <c r="C181" t="s">
+        <v>791</v>
+      </c>
+      <c r="D181" s="1">
+        <v>32176</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182">
         <f t="shared" si="4"/>
-        <v>148</v>
-      </c>
-      <c r="B149" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
+        <v>616</v>
+      </c>
+      <c r="C182" t="s">
+        <v>792</v>
+      </c>
+      <c r="D182" s="1">
+        <v>38596</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183">
         <f t="shared" si="4"/>
-        <v>149</v>
-      </c>
-      <c r="B150" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151">
-        <f t="shared" ref="A151:A207" si="5">A150+1</f>
-        <v>150</v>
-      </c>
-      <c r="B151" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152">
-        <f t="shared" si="5"/>
-        <v>151</v>
-      </c>
-      <c r="B152" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153">
-        <f t="shared" si="5"/>
-        <v>152</v>
-      </c>
-      <c r="B153" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154">
-        <f t="shared" si="5"/>
-        <v>153</v>
-      </c>
-      <c r="B154" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155">
-        <f t="shared" si="5"/>
-        <v>154</v>
-      </c>
-      <c r="B155" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156">
-        <f t="shared" si="5"/>
-        <v>155</v>
-      </c>
-      <c r="B156" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157">
-        <f t="shared" si="5"/>
-        <v>156</v>
-      </c>
-      <c r="B157" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158">
-        <f t="shared" si="5"/>
-        <v>157</v>
-      </c>
-      <c r="B158" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159">
-        <f t="shared" si="5"/>
-        <v>158</v>
-      </c>
-      <c r="B159" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160">
-        <f t="shared" si="5"/>
-        <v>159</v>
-      </c>
-      <c r="B160" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161">
-        <f t="shared" si="5"/>
-        <v>160</v>
-      </c>
-      <c r="B161" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162">
-        <f t="shared" si="5"/>
-        <v>161</v>
-      </c>
-      <c r="B162" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163">
-        <f t="shared" si="5"/>
-        <v>162</v>
-      </c>
-      <c r="B163" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164">
-        <f t="shared" si="5"/>
-        <v>163</v>
-      </c>
-      <c r="B164" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165">
-        <f t="shared" si="5"/>
-        <v>164</v>
-      </c>
-      <c r="B165" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166">
-        <f t="shared" si="5"/>
-        <v>165</v>
-      </c>
-      <c r="B166" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167">
-        <f t="shared" si="5"/>
-        <v>166</v>
-      </c>
-      <c r="B167" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168">
-        <f t="shared" si="5"/>
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169">
-        <f t="shared" si="5"/>
-        <v>168</v>
-      </c>
-      <c r="B169" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170">
-        <f t="shared" si="5"/>
-        <v>169</v>
-      </c>
-      <c r="B170" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171">
-        <f t="shared" si="5"/>
-        <v>170</v>
-      </c>
-      <c r="B171" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172">
-        <f t="shared" si="5"/>
-        <v>171</v>
-      </c>
-      <c r="B172" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173">
-        <f t="shared" si="5"/>
-        <v>172</v>
-      </c>
-      <c r="B173" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174">
-        <f t="shared" si="5"/>
-        <v>173</v>
-      </c>
-      <c r="B174" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175">
-        <f t="shared" si="5"/>
-        <v>174</v>
-      </c>
-      <c r="B175" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176">
-        <f t="shared" si="5"/>
-        <v>175</v>
-      </c>
-      <c r="B176" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177">
-        <f t="shared" si="5"/>
-        <v>176</v>
-      </c>
-      <c r="B177" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178">
-        <f t="shared" si="5"/>
-        <v>177</v>
-      </c>
-      <c r="B178" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179">
-        <f t="shared" si="5"/>
-        <v>178</v>
-      </c>
-      <c r="B179" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180">
-        <f t="shared" si="5"/>
-        <v>179</v>
-      </c>
-      <c r="B180" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181">
-        <f t="shared" si="5"/>
-        <v>180</v>
-      </c>
-      <c r="B181" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182">
-        <f t="shared" si="5"/>
-        <v>181</v>
-      </c>
-      <c r="B182" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183">
-        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+        <v>620</v>
+      </c>
+      <c r="C183" t="s">
+        <v>684</v>
+      </c>
+      <c r="D183" s="1">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+        <v>622</v>
+      </c>
+      <c r="C184" t="s">
+        <v>793</v>
+      </c>
+      <c r="D184" s="1">
+        <v>35704</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+        <v>624</v>
+      </c>
+      <c r="C185" t="s">
+        <v>794</v>
+      </c>
+      <c r="D185" s="1">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+        <v>626</v>
+      </c>
+      <c r="C186" t="s">
+        <v>774</v>
+      </c>
+      <c r="D186" s="1">
+        <v>35781</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+        <v>632</v>
+      </c>
+      <c r="C187" t="s">
+        <v>795</v>
+      </c>
+      <c r="D187" s="1">
+        <v>31686</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+        <v>634</v>
+      </c>
+      <c r="C188" t="s">
+        <v>796</v>
+      </c>
+      <c r="D188" s="1">
+        <v>35781</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+        <v>636</v>
+      </c>
+      <c r="C189" t="s">
+        <v>797</v>
+      </c>
+      <c r="D189" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+        <v>638</v>
+      </c>
+      <c r="C190" t="s">
+        <v>798</v>
+      </c>
+      <c r="D190" s="1">
+        <v>34899</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+        <v>640</v>
+      </c>
+      <c r="C191" t="s">
+        <v>799</v>
+      </c>
+      <c r="D191" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+        <v>642</v>
+      </c>
+      <c r="C192" t="s">
+        <v>710</v>
+      </c>
+      <c r="D192" s="1">
+        <v>1997</v>
+      </c>
+      <c r="E192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+        <v>644</v>
+      </c>
+      <c r="C193" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+        <v>646</v>
+      </c>
+      <c r="C194" t="s">
+        <v>800</v>
+      </c>
+      <c r="D194" s="1">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+        <v>649</v>
+      </c>
+      <c r="C195" t="s">
+        <v>792</v>
+      </c>
+      <c r="D195" s="1">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+        <v>651</v>
+      </c>
+      <c r="C196" t="s">
+        <v>801</v>
+      </c>
+      <c r="D196" s="1">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+        <v>653</v>
+      </c>
+      <c r="C197" t="s">
+        <v>688</v>
+      </c>
+      <c r="D197" s="1">
+        <v>39364</v>
+      </c>
+      <c r="E197" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+        <v>658</v>
+      </c>
+      <c r="C198" t="s">
+        <v>802</v>
+      </c>
+      <c r="D198" s="1">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+        <v>660</v>
+      </c>
+      <c r="C199" t="s">
+        <v>803</v>
+      </c>
+      <c r="D199" s="1">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+        <v>662</v>
+      </c>
+      <c r="C200" t="s">
+        <v>804</v>
+      </c>
+      <c r="D200" s="1">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+        <v>667</v>
+      </c>
+      <c r="C201" t="s">
+        <v>684</v>
+      </c>
+      <c r="D201" s="1">
+        <v>37681</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203">
-        <f t="shared" si="5"/>
-        <v>202</v>
-      </c>
-      <c r="B203" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204">
-        <f t="shared" si="5"/>
-        <v>203</v>
-      </c>
-      <c r="B204" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205">
-        <f t="shared" si="5"/>
-        <v>204</v>
-      </c>
-      <c r="B205" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206">
-        <f t="shared" si="5"/>
-        <v>205</v>
-      </c>
-      <c r="B206" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207">
-        <f t="shared" si="5"/>
-        <v>206</v>
-      </c>
-      <c r="B207" t="s">
-        <v>672</v>
+        <v>670</v>
+      </c>
+      <c r="C202" t="s">
+        <v>805</v>
+      </c>
+      <c r="D202" s="1">
+        <v>33942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>